<commit_message>
Update after finishing schedule for Fall 2023
Removed unnecessary conflicts for professor teaching multiple asynchronous courses.
</commit_message>
<xml_diff>
--- a/Generate Time Codes.xlsx
+++ b/Generate Time Codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/CourseScheduling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2023 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81E90A59-6E8F-4BD4-BCD1-0E4737D5DB68}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C7C7CB4-FF8E-421F-AA8D-815CF055F64A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
   </bookViews>
@@ -36,8 +36,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Calvin Berggren</author>
+  </authors>
+  <commentList>
+    <comment ref="E48" authorId="0" shapeId="0" xr:uid="{B30C7F0B-89AE-4215-9125-DC1BAC993F29}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>it has been 2:30-4:30 some semesters, but Mike said (2/13/2023) always make it 2:30-4:00</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="111">
   <si>
     <t>days</t>
   </si>
@@ -321,9 +345,6 @@
     <t>3:30PM</t>
   </si>
   <si>
-    <t>F2:30-4:30</t>
-  </si>
-  <si>
     <t>M2:30-4:30</t>
   </si>
   <si>
@@ -352,19 +373,47 @@
   </si>
   <si>
     <t>M1-5;T1-5;W1-5;R1-5</t>
+  </si>
+  <si>
+    <t>TWR</t>
+  </si>
+  <si>
+    <t>F2:30-4:00</t>
+  </si>
+  <si>
+    <t>T1-4;W1-4;R1-4</t>
+  </si>
+  <si>
+    <t>ASY</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>M1-5;T1-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -394,7 +443,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -409,21 +465,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -439,8 +481,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E117" totalsRowShown="0">
-  <autoFilter ref="A1:E117" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E121" totalsRowShown="0">
+  <autoFilter ref="A1:E121" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D6A4C193-C770-4795-BA4D-6659D41683A3}" name="days"/>
     <tableColumn id="2" xr3:uid="{E9079B6B-65A1-4117-9DF9-19A5E92BBBAE}" name="begin_time"/>
@@ -448,7 +490,7 @@
     <tableColumn id="4" xr3:uid="{F5DB56F5-5374-46A5-9F52-C165E95C7EB2}" name="merged_daytime" dataDxfId="4">
       <calculatedColumnFormula>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{777DE3F8-1FE5-4C45-8E8A-95849F198C19}" name="timecode" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{777DE3F8-1FE5-4C45-8E8A-95849F198C19}" name="timecode" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -457,8 +499,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}" name="TimeCodeMap" displayName="TimeCodeMap" ref="A1:E56" totalsRowShown="0">
-  <autoFilter ref="A1:E56" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}" name="TimeCodeMap" displayName="TimeCodeMap" ref="A1:E59" totalsRowShown="0">
+  <autoFilter ref="A1:E59" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3F488AE9-9DAA-41D9-8438-57EADAD189CE}" name="merged_daytime" dataDxfId="2">
       <calculatedColumnFormula>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</calculatedColumnFormula>
@@ -769,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71782CAC-D457-4B7E-93F1-D92D90D65B94}">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,60 +843,51 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E2" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D3" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>T6:00PM9:00PM</v>
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>T6-9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D4" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E4" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -862,18 +895,18 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E5" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -881,23 +914,23 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D6" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E6" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -907,16 +940,16 @@
       </c>
       <c r="D7" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E7" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -926,16 +959,16 @@
       </c>
       <c r="D8" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E8" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -945,30 +978,30 @@
       </c>
       <c r="D9" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E9" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D10" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E10" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -976,18 +1009,18 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E11" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -995,56 +1028,47 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D12" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E12" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
       <c r="D13" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v/>
       </c>
       <c r="E13" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D14" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E14" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1068,40 +1092,40 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D16" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E16" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D17" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E17" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>MWF8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1128,61 +1152,61 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D19" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E19" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D20" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E20" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D21" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E21" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1192,73 +1216,73 @@
       </c>
       <c r="D22" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E22" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="D23" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>T9:30AM12:30PM</v>
       </c>
       <c r="E23" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>T9:30-12:30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D24" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E24" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="D25" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>R9:30AM12:30PM</v>
       </c>
       <c r="E25" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>R9:30-12:30</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
@@ -1268,16 +1292,16 @@
       </c>
       <c r="D26" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E26" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -1287,201 +1311,156 @@
       </c>
       <c r="D27" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E27" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D28" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM2:50PM</v>
+        <v>MWF</v>
       </c>
       <c r="E28" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1-2:50</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D29" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E29" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="D30" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>F1:00PM3:00PM</v>
       </c>
       <c r="E30" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>F1-3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D31" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E31" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="D32" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>no8</v>
       </c>
       <c r="E32" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWFno8</v>
+      </c>
+      <c r="E33" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9;MWF10:30;MWF11:30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E34" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
         <v>5</v>
       </c>
-      <c r="D33" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
-      </c>
-      <c r="E33" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
-      </c>
-      <c r="E34" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
       <c r="D35" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW10:30AM11:20AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E35" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW10:30</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D36" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>F1:00PM2:50PM</v>
       </c>
       <c r="E36" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>F1-2:50</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
       <c r="D37" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E37" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1489,137 +1468,104 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D38" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E38" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MWF8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>15</v>
-      </c>
       <c r="D39" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v/>
       </c>
       <c r="E39" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D40" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>TR8:00AM9:15AM</v>
       </c>
       <c r="E40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>TR8</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="D41" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>no8</v>
       </c>
       <c r="E41" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" t="s">
-        <v>5</v>
-      </c>
       <c r="D42" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E42" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" t="s">
-        <v>20</v>
-      </c>
       <c r="D43" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v/>
       </c>
       <c r="E43" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D44" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E44" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
@@ -1629,16 +1575,16 @@
       </c>
       <c r="D45" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E45" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
@@ -1648,284 +1594,239 @@
       </c>
       <c r="D46" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>R1:00PM4:00PM</v>
+      </c>
+      <c r="E46" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>R1-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E47" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>T1:00PM4:00PM</v>
       </c>
-      <c r="E46" t="str">
+      <c r="E48" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>T1-4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
-      </c>
-      <c r="E47" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" t="s">
-        <v>25</v>
-      </c>
-      <c r="D48" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM5:00PM</v>
-      </c>
-      <c r="E48" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5;W1-5;R1-5</v>
-      </c>
-    </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" t="s">
-        <v>25</v>
-      </c>
       <c r="D49" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM5:00PM</v>
+        <v/>
       </c>
       <c r="E49" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-5</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D50" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E50" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>3</v>
-      </c>
       <c r="B51" t="s">
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D51" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM5:00PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E51" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D52" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:30PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E52" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F2:30-4:30</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>21</v>
-      </c>
       <c r="B53" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D53" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:30PM</v>
+        <v>1:00PM5:00PM</v>
       </c>
       <c r="E53" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F2:30-4:30</v>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>12</v>
-      </c>
       <c r="B54" t="s">
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D54" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>1:00PM5:00PM</v>
       </c>
       <c r="E54" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D55" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E55" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D56" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MT1:00PM5:00PM</v>
       </c>
       <c r="E56" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>M1-5;T1-5</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s">
-        <v>8</v>
-      </c>
       <c r="D57" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v/>
       </c>
       <c r="E57" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
       <c r="D58" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>1:00PM5:00PM</v>
       </c>
       <c r="E58" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
         <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="D59" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
+        <v>F2:30PM4:00PM</v>
       </c>
       <c r="E59" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
+        <v>F2:30-4:00</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>14</v>
-      </c>
-      <c r="B60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="D60" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>ASY</v>
       </c>
       <c r="E60" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>ASY</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>14</v>
-      </c>
-      <c r="B61" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" t="s">
-        <v>16</v>
-      </c>
       <c r="D61" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v/>
       </c>
       <c r="E61" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1949,21 +1850,15 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="D63" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v>ASY</v>
       </c>
       <c r="E63" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>ASY</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1971,18 +1866,18 @@
         <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D64" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E64" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2009,66 +1904,75 @@
         <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D66" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E66" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D67" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E67" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MW1:00PM2:15PM</v>
+      </c>
+      <c r="E68" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MW1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>6</v>
       </c>
-      <c r="B68" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
-      </c>
-      <c r="E68" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" t="s">
+        <v>11</v>
+      </c>
       <c r="D69" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E69" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2076,341 +1980,323 @@
         <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D70" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E70" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D71" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E71" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C72" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D72" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>M2:30PM4:30PM</v>
       </c>
       <c r="E72" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>M2:30-4:30</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>24</v>
-      </c>
-      <c r="B73" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="D73" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v>ASY</v>
       </c>
       <c r="E73" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>ASY</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D74" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E74" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C75" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D75" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW2:30PM3:45PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E75" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW2:30</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>14</v>
-      </c>
-      <c r="B76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="D76" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>ASY</v>
       </c>
       <c r="E76" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>ASY</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B77" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D77" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T2:30PM3:20PM</v>
+        <v>TR8:00AM9:15AM</v>
       </c>
       <c r="E77" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T2:30-3:20</v>
+        <v>TR8</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C78" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D78" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>TR2:30PM3:45PM</v>
       </c>
       <c r="E78" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>TR2:30</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D79" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>TR8:00AM9:15AM</v>
       </c>
       <c r="E79" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>TR8</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>6</v>
-      </c>
-      <c r="B80" t="s">
-        <v>7</v>
-      </c>
-      <c r="C80" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="D80" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>ASY</v>
       </c>
       <c r="E80" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>ASY</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C81" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D81" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v>T8:00AM8:50AM</v>
       </c>
       <c r="E81" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>T8</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C82" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D82" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>W2:30PM3:20PM</v>
       </c>
       <c r="E82" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>W2:30-3:20</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C83" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D83" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E83" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C84" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D84" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW11:30AM12:45PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E84" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW11:30-12:45</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D85" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E85" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B86" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D86" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v>MW1:00PM2:15PM</v>
       </c>
       <c r="E86" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>MW1</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C87" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D87" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF1:00PM2:10PM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E87" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF1-2:10</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2418,18 +2304,18 @@
         <v>14</v>
       </c>
       <c r="B88" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D88" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E88" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2437,37 +2323,37 @@
         <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C89" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D89" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>TR2:30PM3:45PM</v>
       </c>
       <c r="E89" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>TR2:30</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D90" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v>MW1:00PM2:15PM</v>
       </c>
       <c r="E90" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>MW1</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2478,298 +2364,310 @@
         <v>7</v>
       </c>
       <c r="C91" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D91" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM12:10PM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E91" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30-12:10</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D92" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM12:10PM</v>
+        <v>MWF11:30AM12:40PM</v>
       </c>
       <c r="E92" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30-12:10</v>
+        <v>MWF11:30-12:40</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B93" t="s">
         <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D93" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>TR10:30AM12:10PM</v>
       </c>
       <c r="E93" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>TR10:30-12:10</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D94" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>MWF11:30AM12:40PM</v>
       </c>
       <c r="E94" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF11:30-12:40</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B95" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C95" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D95" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v>TR10:30AM12:10PM</v>
       </c>
       <c r="E95" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>TR10:30-12:10</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>6</v>
       </c>
+      <c r="B96" t="s">
+        <v>19</v>
+      </c>
+      <c r="C96" t="s">
+        <v>31</v>
+      </c>
       <c r="D96" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v>MWF11:30AM12:40PM</v>
       </c>
       <c r="E96" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
+        <v>MWF11:30-12:40</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="D97" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
+        <v>no8</v>
       </c>
       <c r="E97" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>14</v>
+      </c>
+      <c r="B98" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s">
+        <v>33</v>
       </c>
       <c r="D98" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
+        <v>TR10:30AM12:10PM</v>
       </c>
       <c r="E98" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30</v>
+        <v>TR10:30-12:10</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>14</v>
+      </c>
+      <c r="B99" t="s">
+        <v>4</v>
+      </c>
+      <c r="C99" t="s">
+        <v>16</v>
       </c>
       <c r="D99" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E99" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>14</v>
-      </c>
-      <c r="B100" t="s">
-        <v>7</v>
-      </c>
-      <c r="C100" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="D100" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E100" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>check</v>
+      </c>
+      <c r="E100" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B101" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C101" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D101" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>F2:30PM4:00PM</v>
       </c>
       <c r="E101" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>F2:30-4:00</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B102" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D102" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E102" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B103" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C103" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D103" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T6:00PM8:30PM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E103" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T6-8:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B104" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D104" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E104" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C105" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D105" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>TR8:00AM9:15AM</v>
       </c>
       <c r="E105" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>TR8</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B106" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C106" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D106" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>TR2:30PM3:45PM</v>
       </c>
       <c r="E106" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>TR2:30</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>24</v>
+      </c>
       <c r="B107" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C107" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D107" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>MW8:00AM8:50AM</v>
       </c>
       <c r="E107" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>MW8</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>9</v>
-      </c>
       <c r="B108" t="s">
         <v>4</v>
       </c>
@@ -2778,55 +2676,40 @@
       </c>
       <c r="D108" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E108" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>6</v>
-      </c>
-      <c r="B109" t="s">
-        <v>7</v>
-      </c>
-      <c r="C109" t="s">
-        <v>20</v>
-      </c>
       <c r="D109" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM12:20PM</v>
+        <v/>
       </c>
       <c r="E109" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30-12:20</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>6</v>
-      </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D110" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E110" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>9</v>
-      </c>
       <c r="B111" t="s">
         <v>4</v>
       </c>
@@ -2835,49 +2718,37 @@
       </c>
       <c r="D111" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E111" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>3</v>
-      </c>
-      <c r="B112" t="s">
-        <v>4</v>
-      </c>
-      <c r="C112" t="s">
+      <c r="D112" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E112" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>4</v>
+      </c>
+      <c r="C113" t="s">
         <v>5</v>
       </c>
-      <c r="D112" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
-      </c>
-      <c r="E112" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>14</v>
-      </c>
-      <c r="B113" t="s">
-        <v>7</v>
-      </c>
-      <c r="C113" t="s">
-        <v>15</v>
-      </c>
       <c r="D113" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E113" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2885,42 +2756,33 @@
         <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C114" t="s">
         <v>20</v>
       </c>
       <c r="D114" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>MWF10:30AM12:20PM</v>
       </c>
       <c r="E114" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>MWF10:30-12:20</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>6</v>
-      </c>
-      <c r="B115" t="s">
-        <v>17</v>
-      </c>
-      <c r="C115" t="s">
-        <v>18</v>
-      </c>
       <c r="D115" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v/>
       </c>
       <c r="E115" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="B116" t="s">
         <v>4</v>
@@ -2930,30 +2792,106 @@
       </c>
       <c r="D116" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>TWR1:00PM4:00PM</v>
       </c>
       <c r="E116" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C117" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D117" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM1:50PM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E117" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1</v>
+        <v>MWF8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>14</v>
+      </c>
+      <c r="B118" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118" s="1" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR10:30AM11:45AM</v>
+      </c>
+      <c r="E118" s="1" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR10:30</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>14</v>
+      </c>
+      <c r="B119" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119" s="1" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR10:30AM11:45AM</v>
+      </c>
+      <c r="E119" s="1" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR10:30</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" t="s">
+        <v>5</v>
+      </c>
+      <c r="D120" s="1" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>R1:00PM4:00PM</v>
+      </c>
+      <c r="E120" s="1" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>R1-4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>14</v>
+      </c>
+      <c r="B121" t="s">
+        <v>17</v>
+      </c>
+      <c r="C121" t="s">
+        <v>23</v>
+      </c>
+      <c r="D121" s="1" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR8:00AM9:15AM</v>
+      </c>
+      <c r="E121" s="1" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8</v>
       </c>
     </row>
   </sheetData>
@@ -2965,10 +2903,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377702D3-3049-4D9F-8497-CBC60EF1DE1E}">
-  <dimension ref="A1:E56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377702D3-3049-4D9F-8497-CBC60EF1DE1E}">
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3824,9 +3764,9 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="str">
-        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:30PM</v>
+      <c r="A48" s="1" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>F2:30PM4:00PM</v>
       </c>
       <c r="B48" t="s">
         <v>21</v>
@@ -3835,10 +3775,10 @@
         <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3856,11 +3796,11 @@
         <v>27</v>
       </c>
       <c r="E49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="str">
+      <c r="A50" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF</v>
       </c>
@@ -3868,11 +3808,11 @@
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="str">
+      <c r="A51" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR</v>
       </c>
@@ -3880,44 +3820,44 @@
         <v>14</v>
       </c>
       <c r="E51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>no8</v>
+      </c>
+      <c r="B53" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="str">
-        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E52" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="str">
-        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
-        <v>no8</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="E53" t="s">
         <v>99</v>
       </c>
-      <c r="E53" t="s">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>MWFno8</v>
+      </c>
+      <c r="B54" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="str">
-        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="E54" t="s">
         <v>101</v>
       </c>
-      <c r="E54" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="str">
+      <c r="A55" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>1:00PM4:00PM</v>
       </c>
@@ -3928,11 +3868,11 @@
         <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="str">
+      <c r="A56" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>1:00PM5:00PM</v>
       </c>
@@ -3943,13 +3883,62 @@
         <v>25</v>
       </c>
       <c r="E56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>TWR1:00PM4:00PM</v>
+      </c>
+      <c r="B57" t="s">
         <v>104</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>MT1:00PM5:00PM</v>
+      </c>
+      <c r="B58" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>ASY</v>
+      </c>
+      <c r="B59" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update after finishing schedule for Spring 2024
</commit_message>
<xml_diff>
--- a/Generate Time Codes.xlsx
+++ b/Generate Time Codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2023 Fall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2024 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C7C7CB4-FF8E-421F-AA8D-815CF055F64A}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34239FFE-A56D-429C-955E-C716B20DFD1F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="131">
   <si>
     <t>days</t>
   </si>
@@ -390,10 +390,70 @@
     <t>MT</t>
   </si>
   <si>
-    <t>check</t>
-  </si>
-  <si>
     <t>M1-5;T1-5</t>
+  </si>
+  <si>
+    <t>MWFmorn</t>
+  </si>
+  <si>
+    <t>Trmorn</t>
+  </si>
+  <si>
+    <t>morn</t>
+  </si>
+  <si>
+    <t>no8morn</t>
+  </si>
+  <si>
+    <t>MWFno8morn</t>
+  </si>
+  <si>
+    <t>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</t>
+  </si>
+  <si>
+    <t>TR8;TR10:30;TR1;TR2:30</t>
+  </si>
+  <si>
+    <t>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</t>
+  </si>
+  <si>
+    <t>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</t>
+  </si>
+  <si>
+    <t>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</t>
+  </si>
+  <si>
+    <t>TRmorn</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>MTW</t>
+  </si>
+  <si>
+    <t>MWF-check</t>
+  </si>
+  <si>
+    <t>TR-check</t>
+  </si>
+  <si>
+    <t>MWFcheck</t>
+  </si>
+  <si>
+    <t>Trcheck</t>
+  </si>
+  <si>
+    <t>Mwcheck</t>
+  </si>
+  <si>
+    <t>8:20PM</t>
+  </si>
+  <si>
+    <t>W1-4;R1-4</t>
+  </si>
+  <si>
+    <t>M1-5;T1-5;W1-5</t>
   </si>
 </sst>
 </file>
@@ -443,14 +503,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -481,16 +534,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E121" totalsRowShown="0">
-  <autoFilter ref="A1:E121" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E116" totalsRowShown="0">
+  <autoFilter ref="A1:E116" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D6A4C193-C770-4795-BA4D-6659D41683A3}" name="days"/>
     <tableColumn id="2" xr3:uid="{E9079B6B-65A1-4117-9DF9-19A5E92BBBAE}" name="begin_time"/>
     <tableColumn id="3" xr3:uid="{91E2F62C-BC78-4486-8262-E8EB91EEAF07}" name="end_time"/>
-    <tableColumn id="4" xr3:uid="{F5DB56F5-5374-46A5-9F52-C165E95C7EB2}" name="merged_daytime" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{F5DB56F5-5374-46A5-9F52-C165E95C7EB2}" name="merged_daytime" dataDxfId="3">
       <calculatedColumnFormula>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{777DE3F8-1FE5-4C45-8E8A-95849F198C19}" name="timecode" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{777DE3F8-1FE5-4C45-8E8A-95849F198C19}" name="timecode" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -499,10 +552,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}" name="TimeCodeMap" displayName="TimeCodeMap" ref="A1:E59" totalsRowShown="0">
-  <autoFilter ref="A1:E59" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}" name="TimeCodeMap" displayName="TimeCodeMap" ref="A1:E67" totalsRowShown="0">
+  <autoFilter ref="A1:E67" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3F488AE9-9DAA-41D9-8438-57EADAD189CE}" name="merged_daytime" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{3F488AE9-9DAA-41D9-8438-57EADAD189CE}" name="merged_daytime" dataDxfId="1">
       <calculatedColumnFormula>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{60CB15DE-0792-4C86-9DA9-F5946FF20273}" name="days"/>
@@ -811,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71782CAC-D457-4B7E-93F1-D92D90D65B94}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E121"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,94 +896,82 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
       <c r="D2" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E2" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="D3" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T6:00PM9:00PM</v>
+        <v>no8morn</v>
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T6-9</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D4" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E4" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="D5" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>MWFmorn</v>
       </c>
       <c r="E5" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="D6" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>MWFmorn</v>
       </c>
       <c r="E6" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -940,16 +981,16 @@
       </c>
       <c r="D7" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E7" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -959,121 +1000,112 @@
       </c>
       <c r="D8" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E8" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="D9" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>TRmorn</v>
       </c>
       <c r="E9" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>TR8;TR10:30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D10" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E10" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D11" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E11" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="D12" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>TRmorn</v>
       </c>
       <c r="E12" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>TR8;TR10:30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
       <c r="D13" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>WR1:00PM4:00PM</v>
       </c>
       <c r="E13" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>W1-4;R1-4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>MWF</v>
       </c>
       <c r="E14" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1083,30 +1115,30 @@
       </c>
       <c r="D15" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E15" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D16" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E16" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>MWF8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1114,18 +1146,18 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D17" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E17" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1133,80 +1165,80 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D18" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E18" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D19" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E19" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D20" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E20" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D21" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E21" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1216,93 +1248,84 @@
       </c>
       <c r="D22" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E22" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="D23" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T9:30AM12:30PM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E23" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T9:30-12:30</v>
+        <v>MWF8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="D24" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>F1:00PM3:00PM</v>
       </c>
       <c r="E24" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>F1-3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="D25" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R9:30AM12:30PM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E25" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R9:30-12:30</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D26" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>MWFno8</v>
       </c>
       <c r="E26" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>9</v>
-      </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
@@ -1311,281 +1334,314 @@
       </c>
       <c r="D27" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E27" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
       </c>
       <c r="D28" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v>F1:00PM2:50PM</v>
       </c>
       <c r="E28" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
+        <v>F1-2:50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
       <c r="D29" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E29" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
-      </c>
       <c r="D30" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM3:00PM</v>
+        <v/>
       </c>
       <c r="E30" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1-3</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
+      <c r="A31" t="s">
+        <v>14</v>
       </c>
       <c r="D31" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>TR</v>
       </c>
       <c r="E31" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D32" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
+        <v>MWFno8</v>
       </c>
       <c r="E32" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30</v>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>M1:00PM4:00PM</v>
+      </c>
+      <c r="E33" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>100</v>
       </c>
-      <c r="D33" t="str">
+      <c r="D34" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>MWFno8</v>
       </c>
-      <c r="E33" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D34" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
       <c r="E34" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D35" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E35" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D36" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM2:50PM</v>
+        <v>MW10:30AM11:20AM</v>
       </c>
       <c r="E36" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1-2:50</v>
+        <v>MW10:30</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>110</v>
+      </c>
       <c r="D37" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>MWFmorn</v>
       </c>
       <c r="E37" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D38" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E38" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
       <c r="D39" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E39" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D40" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
       </c>
       <c r="D41" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E41" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
       <c r="D42" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E42" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
       <c r="D43" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E43" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D44" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E44" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>MWF8</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D45" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E45" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
@@ -1594,216 +1650,225 @@
       </c>
       <c r="D46" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E46" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
       <c r="D47" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E47" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D48" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E48" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
       <c r="D49" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>M1:00PM5:00PM</v>
       </c>
       <c r="E49" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>M1-5</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
       <c r="B50" t="s">
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D50" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>W1:00PM5:00PM</v>
       </c>
       <c r="E50" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>W1-5</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" t="s">
-        <v>5</v>
+      <c r="A51" t="s">
+        <v>100</v>
       </c>
       <c r="D51" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>MWFno8</v>
       </c>
       <c r="E51" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MTW1:00PM5:00PM</v>
+      </c>
+      <c r="E52" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-5;T1-5;W1-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>6</v>
       </c>
-      <c r="B52" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
-      </c>
-      <c r="E52" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" t="s">
-        <v>25</v>
-      </c>
       <c r="D53" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM5:00PM</v>
+        <v>MWF</v>
       </c>
       <c r="E53" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5;W1-5;R1-5</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D54" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM5:00PM</v>
+        <v>F2:30PM4:00PM</v>
       </c>
       <c r="E54" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5;W1-5;R1-5</v>
+        <v>F2:30-4:00</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>F2:30PM4:00PM</v>
+      </c>
+      <c r="E55" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>F2:30-4:00</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E56" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>14</v>
       </c>
-      <c r="B55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E55" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>108</v>
-      </c>
-      <c r="B56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C56" t="s">
-        <v>25</v>
-      </c>
-      <c r="D56" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MT1:00PM5:00PM</v>
-      </c>
-      <c r="E56" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D57" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR</v>
+      </c>
+      <c r="E57" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D58" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E57" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM5:00PM</v>
-      </c>
       <c r="E58" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5;W1-5;R1-5</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D59" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:00PM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E59" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F2:30-4:00</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1826,101 +1891,83 @@
       </c>
       <c r="E61" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D62" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E62" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>14</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" t="s">
+        <v>16</v>
       </c>
       <c r="D63" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>ASY</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E63" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>ASY</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>6</v>
-      </c>
-      <c r="B64" t="s">
-        <v>19</v>
-      </c>
-      <c r="C64" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D64" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>MWFno8</v>
       </c>
       <c r="E64" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>14</v>
-      </c>
-      <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s">
-        <v>15</v>
-      </c>
       <c r="D65" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v/>
       </c>
       <c r="E65" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s">
-        <v>8</v>
-      </c>
       <c r="D66" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v/>
       </c>
       <c r="E66" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
@@ -1930,170 +1977,149 @@
       </c>
       <c r="D67" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
-      </c>
-      <c r="E67" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF-check10:30AM11:20AM</v>
+      </c>
+      <c r="E67" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>24</v>
-      </c>
-      <c r="B68" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="D68" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v>ASY</v>
       </c>
       <c r="E68" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>ASY</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D69" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E69" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D70" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E70" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C71" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D71" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>TR8:00AM9:15AM</v>
       </c>
       <c r="E71" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>TR8</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D72" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M2:30PM4:30PM</v>
-      </c>
-      <c r="E72" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M2:30-4:30</v>
+        <v>TR-check10:30AM11:45AM</v>
+      </c>
+      <c r="E72" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>107</v>
-      </c>
       <c r="D73" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>ASY</v>
+        <v/>
       </c>
       <c r="E73" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>ASY</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74" t="s">
-        <v>16</v>
-      </c>
       <c r="D74" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v/>
       </c>
       <c r="E74" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" t="s">
-        <v>10</v>
-      </c>
-      <c r="C75" t="s">
-        <v>11</v>
-      </c>
       <c r="D75" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v/>
       </c>
       <c r="E75" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>107</v>
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" t="s">
+        <v>11</v>
       </c>
       <c r="D76" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>ASY</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E76" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>ASY</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2101,335 +2127,302 @@
         <v>14</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D77" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E77" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C78" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D78" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E78" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D79" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E79" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>24</v>
+      </c>
+      <c r="B80" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" t="s">
+        <v>16</v>
       </c>
       <c r="D80" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>ASY</v>
+        <v>MW1:00PM2:15PM</v>
       </c>
       <c r="E80" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>ASY</v>
+        <v>MW1</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B81" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D81" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T8:00AM8:50AM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E81" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T8</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D82" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W2:30PM3:20PM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E82" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W2:30-3:20</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D83" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E83" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>6</v>
-      </c>
-      <c r="B84" t="s">
-        <v>10</v>
-      </c>
-      <c r="C84" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="D84" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>no8</v>
       </c>
       <c r="E84" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C85" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D85" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
-      </c>
-      <c r="E85" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWFcheck11:30AM12:40PM</v>
+      </c>
+      <c r="E85" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>24</v>
-      </c>
-      <c r="B86" t="s">
-        <v>4</v>
-      </c>
-      <c r="C86" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="D86" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v>no8</v>
       </c>
       <c r="E86" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>14</v>
       </c>
-      <c r="B87" t="s">
-        <v>7</v>
-      </c>
-      <c r="C87" t="s">
-        <v>15</v>
-      </c>
       <c r="D87" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>TR</v>
       </c>
       <c r="E87" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D88" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>MWF11:30AM12:40PM</v>
       </c>
       <c r="E88" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF11:30-12:40</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D89" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
+        <v>MWF1:00PM2:10PM</v>
       </c>
       <c r="E89" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
+        <v>MWF1-2:10</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C90" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D90" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
-      </c>
-      <c r="E90" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>Trcheck10:30AM12:10PM</v>
+      </c>
+      <c r="E90" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D91" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E91" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>Mwcheck1:00PM2:15PM</v>
+      </c>
+      <c r="E91" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>6</v>
-      </c>
-      <c r="B92" t="s">
-        <v>19</v>
-      </c>
-      <c r="C92" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="D92" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v>no8</v>
       </c>
       <c r="E92" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>14</v>
-      </c>
-      <c r="B93" t="s">
-        <v>7</v>
-      </c>
-      <c r="C93" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="D93" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM12:10PM</v>
+        <v>MWFno8</v>
       </c>
       <c r="E93" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30-12:10</v>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>6</v>
-      </c>
-      <c r="B94" t="s">
-        <v>19</v>
-      </c>
-      <c r="C94" t="s">
-        <v>31</v>
-      </c>
       <c r="D94" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v/>
       </c>
       <c r="E94" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2437,18 +2430,18 @@
         <v>14</v>
       </c>
       <c r="B95" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D95" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM12:10PM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E95" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30-12:10</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2456,31 +2449,37 @@
         <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C96" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D96" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E96" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>6</v>
+      </c>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
       </c>
       <c r="D97" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E97" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2488,183 +2487,150 @@
         <v>14</v>
       </c>
       <c r="B98" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C98" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D98" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM12:10PM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E98" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30-12:10</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>14</v>
-      </c>
-      <c r="B99" t="s">
-        <v>4</v>
-      </c>
-      <c r="C99" t="s">
-        <v>16</v>
-      </c>
       <c r="D99" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v/>
       </c>
       <c r="E99" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>14</v>
+      </c>
+      <c r="B100" t="s">
+        <v>26</v>
+      </c>
+      <c r="C100" t="s">
+        <v>28</v>
       </c>
       <c r="D100" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>check</v>
-      </c>
-      <c r="E100" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>TR2:30PM3:45PM</v>
+      </c>
+      <c r="E100" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR2:30</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B101" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C101" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="D101" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:00PM</v>
-      </c>
-      <c r="E101" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F2:30-4:00</v>
+        <v>T6:00PM8:20PM</v>
+      </c>
+      <c r="E101" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>6</v>
       </c>
-      <c r="B102" t="s">
-        <v>19</v>
-      </c>
-      <c r="C102" t="s">
-        <v>20</v>
-      </c>
       <c r="D102" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>MWF</v>
       </c>
       <c r="E102" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>6</v>
-      </c>
       <c r="B103" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D103" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E103" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>14</v>
-      </c>
-      <c r="B104" t="s">
-        <v>4</v>
-      </c>
-      <c r="C104" t="s">
-        <v>16</v>
-      </c>
       <c r="D104" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v/>
       </c>
       <c r="E104" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>14</v>
-      </c>
       <c r="B105" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C105" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D105" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E105" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C106" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D106" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
+        <v>MWF10:30AM12:20PM</v>
       </c>
       <c r="E106" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
+        <v>MWF10:30-12:20</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>24</v>
-      </c>
-      <c r="B107" t="s">
-        <v>17</v>
-      </c>
-      <c r="C107" t="s">
-        <v>18</v>
-      </c>
       <c r="D107" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW8:00AM8:50AM</v>
+        <v/>
       </c>
       <c r="E107" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW8</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2684,214 +2650,119 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
       <c r="D109" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E109" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D110" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E109" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>4</v>
-      </c>
-      <c r="C110" t="s">
+      <c r="E110" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111" t="s">
+        <v>18</v>
+      </c>
+      <c r="D111" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF8:00AM8:50AM</v>
+      </c>
+      <c r="E111" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>110</v>
+      </c>
+      <c r="D112" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWFmorn</v>
+      </c>
+      <c r="E112" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D113" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E113" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+      <c r="C114" t="s">
         <v>5</v>
       </c>
-      <c r="D110" t="str">
+      <c r="D114" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>1:00PM4:00PM</v>
       </c>
-      <c r="E110" t="str">
+      <c r="E114" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>4</v>
-      </c>
-      <c r="C111" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E111" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D112" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E112" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>4</v>
-      </c>
-      <c r="C113" t="s">
-        <v>5</v>
-      </c>
-      <c r="D113" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E113" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>6</v>
-      </c>
-      <c r="B114" t="s">
-        <v>7</v>
-      </c>
-      <c r="C114" t="s">
-        <v>20</v>
-      </c>
-      <c r="D114" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM12:20PM</v>
-      </c>
-      <c r="E114" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30-12:20</v>
-      </c>
-    </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>14</v>
+      </c>
       <c r="D115" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>TR</v>
       </c>
       <c r="E115" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>104</v>
+        <v>21</v>
       </c>
       <c r="B116" t="s">
         <v>4</v>
       </c>
       <c r="C116" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D116" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TWR1:00PM4:00PM</v>
+        <v>F1:00PM1:50PM</v>
       </c>
       <c r="E116" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>6</v>
-      </c>
-      <c r="B117" t="s">
-        <v>17</v>
-      </c>
-      <c r="C117" t="s">
-        <v>18</v>
-      </c>
-      <c r="D117" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
-      </c>
-      <c r="E117" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>14</v>
-      </c>
-      <c r="B118" t="s">
-        <v>7</v>
-      </c>
-      <c r="C118" t="s">
-        <v>15</v>
-      </c>
-      <c r="D118" s="1" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E118" s="1" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>14</v>
-      </c>
-      <c r="B119" t="s">
-        <v>7</v>
-      </c>
-      <c r="C119" t="s">
-        <v>15</v>
-      </c>
-      <c r="D119" s="1" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E119" s="1" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>9</v>
-      </c>
-      <c r="B120" t="s">
-        <v>4</v>
-      </c>
-      <c r="C120" t="s">
-        <v>5</v>
-      </c>
-      <c r="D120" s="1" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
-      </c>
-      <c r="E120" s="1" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>14</v>
-      </c>
-      <c r="B121" t="s">
-        <v>17</v>
-      </c>
-      <c r="C121" t="s">
-        <v>23</v>
-      </c>
-      <c r="D121" s="1" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
-      </c>
-      <c r="E121" s="1" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>F1</v>
       </c>
     </row>
   </sheetData>
@@ -2904,10 +2775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377702D3-3049-4D9F-8497-CBC60EF1DE1E}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3764,7 +3635,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="str">
+      <c r="A48" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F2:30PM4:00PM</v>
       </c>
@@ -3808,7 +3679,7 @@
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3820,7 +3691,7 @@
         <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3829,7 +3700,7 @@
         <v/>
       </c>
       <c r="E52" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3841,7 +3712,7 @@
         <v>98</v>
       </c>
       <c r="E53" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3853,84 +3724,192 @@
         <v>100</v>
       </c>
       <c r="E54" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="str">
-        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="C55" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" t="s">
-        <v>5</v>
+      <c r="A55" s="1" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>MWFmorn</v>
+      </c>
+      <c r="B55" t="s">
+        <v>110</v>
       </c>
       <c r="E55" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="str">
-        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
-        <v>1:00PM5:00PM</v>
-      </c>
-      <c r="C56" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" t="s">
-        <v>25</v>
+      <c r="A56" s="1" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>TRmorn</v>
+      </c>
+      <c r="B56" t="s">
+        <v>120</v>
       </c>
       <c r="E56" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
-        <v>TWR1:00PM4:00PM</v>
+        <v>Trmorn</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="E57" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
-        <v>MT1:00PM5:00PM</v>
+        <v>morn</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
-      </c>
-      <c r="C58" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="E58" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>no8morn</v>
+      </c>
+      <c r="B59" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>MWFno8morn</v>
+      </c>
+      <c r="B60" t="s">
+        <v>114</v>
+      </c>
+      <c r="E60" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>1:00PM5:00PM</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>TWR1:00PM4:00PM</v>
+      </c>
+      <c r="B63" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>WR1:00PM4:00PM</v>
+      </c>
+      <c r="B64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>MT1:00PM5:00PM</v>
+      </c>
+      <c r="B65" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
+        <v>MTW1:00PM5:00PM</v>
+      </c>
+      <c r="B66" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>ASY</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B67" t="s">
         <v>107</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E67" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update after finishing schedule for Fall 2024
</commit_message>
<xml_diff>
--- a/Generate Time Codes.xlsx
+++ b/Generate Time Codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2024 Spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2024 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34239FFE-A56D-429C-955E-C716B20DFD1F}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71C9FAE9-8D5E-4453-9BBF-BC1B8084328E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="126">
   <si>
     <t>days</t>
   </si>
@@ -432,28 +432,13 @@
     <t>MTW</t>
   </si>
   <si>
-    <t>MWF-check</t>
-  </si>
-  <si>
-    <t>TR-check</t>
-  </si>
-  <si>
-    <t>MWFcheck</t>
-  </si>
-  <si>
-    <t>Trcheck</t>
-  </si>
-  <si>
-    <t>Mwcheck</t>
-  </si>
-  <si>
-    <t>8:20PM</t>
-  </si>
-  <si>
     <t>W1-4;R1-4</t>
   </si>
   <si>
     <t>M1-5;T1-5;W1-5</t>
+  </si>
+  <si>
+    <t>check</t>
   </si>
 </sst>
 </file>
@@ -534,8 +519,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E116" totalsRowShown="0">
-  <autoFilter ref="A1:E116" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E117" totalsRowShown="0">
+  <autoFilter ref="A1:E117" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D6A4C193-C770-4795-BA4D-6659D41683A3}" name="days"/>
     <tableColumn id="2" xr3:uid="{E9079B6B-65A1-4117-9DF9-19A5E92BBBAE}" name="begin_time"/>
@@ -864,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71782CAC-D457-4B7E-93F1-D92D90D65B94}">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E116"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,81 +882,102 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="D2" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>MW6:00PM7:30PM</v>
       </c>
       <c r="E2" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>MW6-7:30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
       </c>
       <c r="D3" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8morn</v>
+        <v>R6:00PM9:00PM</v>
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30</v>
+        <v>R6-9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D4" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E4" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
       <c r="D5" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFmorn</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E5" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
       </c>
       <c r="D6" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFmorn</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E6" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -981,16 +987,16 @@
       </c>
       <c r="D7" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E7" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1000,107 +1006,113 @@
       </c>
       <c r="D8" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E8" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
       </c>
       <c r="D9" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TRmorn</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E9" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D10" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E10" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D11" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
-      </c>
-      <c r="E11" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MW8:00AM</v>
+      </c>
+      <c r="E11" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
       </c>
       <c r="D12" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TRmorn</v>
+        <v>MW2:30PM3:45PM</v>
       </c>
       <c r="E12" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30</v>
+        <v>MW2:30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D13" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>WR1:00PM4:00PM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E13" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4;R1-4</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
       <c r="D14" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v/>
       </c>
       <c r="E14" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1124,40 +1136,40 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D16" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E16" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D17" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E17" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,80 +1177,80 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E18" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>MWF8</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D19" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E19" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D20" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E20" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D21" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E21" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1248,54 +1260,54 @@
       </c>
       <c r="D22" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E22" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="D23" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>T9:30AM12:30PM</v>
       </c>
       <c r="E23" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
+        <v>T9:30-12:30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="D24" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM3:00PM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E24" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1-3</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
@@ -1305,27 +1317,36 @@
       </c>
       <c r="D25" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E25" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
       </c>
       <c r="D26" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
+        <v>R9:30AM12:30PM</v>
       </c>
       <c r="E26" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>R9:30-12:30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
@@ -1334,311 +1355,296 @@
       </c>
       <c r="D27" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E27" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>morn</v>
+      </c>
+      <c r="E28" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E29" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>21</v>
       </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM2:50PM</v>
-      </c>
-      <c r="E28" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1-2:50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D29" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E29" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
       <c r="D30" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>F1:00PM3:00PM</v>
       </c>
       <c r="E30" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>F1-3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>14</v>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
       </c>
       <c r="D31" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E31" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30;TR1;TR2:30</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D32" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
+        <v>no8</v>
       </c>
       <c r="E32" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D33" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>MWFno8</v>
       </c>
       <c r="E33" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>100</v>
-      </c>
       <c r="D34" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
+        <v/>
       </c>
       <c r="E34" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D35" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E35" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>check1:00PM4:00PM</v>
+      </c>
+      <c r="E35" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D36" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW10:30AM11:20AM</v>
+        <v>F1:00PM2:50PM</v>
       </c>
       <c r="E36" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW10:30</v>
+        <v>F1-2:50</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>110</v>
-      </c>
       <c r="D37" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFmorn</v>
+        <v/>
       </c>
       <c r="E37" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D38" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E38" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>MWF8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>15</v>
-      </c>
       <c r="D39" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v/>
       </c>
       <c r="E39" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D40" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>TR8:00AM9:15AM</v>
       </c>
       <c r="E40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>TR8</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D41" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E41" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D42" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E42" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR10:30AM11:20AM</v>
+      </c>
+      <c r="E43" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
         <v>5</v>
       </c>
-      <c r="D43" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
-      </c>
-      <c r="E43" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>18</v>
-      </c>
       <c r="D44" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E44" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>6</v>
-      </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D45" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E45" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1658,230 +1664,218 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D47" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E47" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
         <v>5</v>
       </c>
-      <c r="D47" t="str">
+      <c r="D48" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>1:00PM4:00PM</v>
       </c>
-      <c r="E47" t="str">
+      <c r="E48" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
-      </c>
-      <c r="E48" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" t="s">
-        <v>25</v>
-      </c>
       <c r="D49" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM5:00PM</v>
+        <v/>
       </c>
       <c r="E49" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>13</v>
-      </c>
       <c r="B50" t="s">
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D50" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM5:00PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E50" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-5</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>100</v>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
       </c>
       <c r="D51" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E51" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF9:00AM9:50AM</v>
+      </c>
+      <c r="E52" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
         <v>25</v>
       </c>
-      <c r="D52" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MTW1:00PM5:00PM</v>
-      </c>
-      <c r="E52" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5;W1-5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>6</v>
-      </c>
       <c r="D53" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v>1:00PM5:00PM</v>
       </c>
       <c r="E53" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>21</v>
-      </c>
       <c r="B54" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D54" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:00PM</v>
+        <v>1:00PM5:00PM</v>
       </c>
       <c r="E54" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F2:30-4:00</v>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="D55" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:00PM</v>
+        <v>no8</v>
       </c>
       <c r="E55" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F2:30-4:00</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
       <c r="B56" t="s">
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D56" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>M1:00PM5:00PM</v>
       </c>
       <c r="E56" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>M1-5</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>14</v>
-      </c>
       <c r="D57" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
+        <v/>
       </c>
       <c r="E57" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30;TR1;TR2:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
       <c r="D58" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>1:00PM5:00PM</v>
       </c>
       <c r="E58" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D59" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>F2:30PM4:00PM</v>
       </c>
       <c r="E59" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>F2:30-4:00</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>107</v>
+        <v>21</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
       </c>
       <c r="D60" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>ASY</v>
+        <v>F2:30PM4:00PM</v>
       </c>
       <c r="E60" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>ASY</v>
+        <v>F2:30-4:00</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1896,230 +1890,263 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D62" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E62" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>14</v>
-      </c>
-      <c r="B63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="D63" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>ASY</v>
       </c>
       <c r="E63" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>ASY</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>14</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
       </c>
       <c r="D64" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
-      </c>
-      <c r="E64" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>TR10:30AM11:20AM</v>
+      </c>
+      <c r="E64" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>11</v>
+      </c>
       <c r="D65" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E65" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>16</v>
+      </c>
       <c r="D66" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>MW1:00PM2:15PM</v>
       </c>
       <c r="E66" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>MW1</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D67" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF-check10:30AM11:20AM</v>
-      </c>
-      <c r="E67" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>TR10:30AM11:45AM</v>
+      </c>
+      <c r="E67" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="D68" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>ASY</v>
-      </c>
-      <c r="E68" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>ASY</v>
+        <v>check</v>
+      </c>
+      <c r="E68" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D69" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E69" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>6</v>
-      </c>
-      <c r="B70" t="s">
-        <v>19</v>
-      </c>
-      <c r="C70" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="D70" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
-      </c>
-      <c r="E70" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>check</v>
+      </c>
+      <c r="E70" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D71" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E71" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D72" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR-check10:30AM11:45AM</v>
-      </c>
-      <c r="E72" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>M2:30PM4:30PM</v>
+      </c>
+      <c r="E72" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M2:30-4:30</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" t="s">
+        <v>16</v>
+      </c>
       <c r="D73" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E73" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" t="s">
+        <v>23</v>
+      </c>
       <c r="D74" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>TR8:00AM9:15AM</v>
       </c>
       <c r="E74" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>TR8</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>107</v>
+      </c>
       <c r="D75" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>ASY</v>
       </c>
       <c r="E75" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>ASY</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>6</v>
-      </c>
-      <c r="B76" t="s">
-        <v>10</v>
-      </c>
-      <c r="C76" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B76">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C76">
+        <v>0.65625</v>
       </c>
       <c r="D76" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
-      </c>
-      <c r="E76" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>TR0.6041666666666670.65625</v>
+      </c>
+      <c r="E76" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2127,364 +2154,349 @@
         <v>14</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D77" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E77" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C78" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D78" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MW2:30PM3:45PM</v>
       </c>
       <c r="E78" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MW2:30</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>6</v>
-      </c>
-      <c r="B79" t="s">
-        <v>7</v>
-      </c>
-      <c r="C79" t="s">
-        <v>8</v>
-      </c>
       <c r="D79" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v/>
       </c>
       <c r="E79" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>24</v>
-      </c>
-      <c r="B80" t="s">
-        <v>4</v>
-      </c>
-      <c r="C80" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="D80" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
-      </c>
-      <c r="E80" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>check</v>
+      </c>
+      <c r="E80" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>14</v>
-      </c>
-      <c r="B81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C81" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="D81" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E81" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>check</v>
+      </c>
+      <c r="E81" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>14</v>
-      </c>
-      <c r="B82" t="s">
-        <v>4</v>
-      </c>
-      <c r="C82" t="s">
-        <v>16</v>
-      </c>
       <c r="D82" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v/>
       </c>
       <c r="E82" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D83" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E83" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>98</v>
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
       </c>
       <c r="D84" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E84" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>125</v>
+        <v>24</v>
       </c>
       <c r="B85" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D85" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFcheck11:30AM12:40PM</v>
-      </c>
-      <c r="E85" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>MW1:00PM2:15PM</v>
+      </c>
+      <c r="E85" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MW1</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>14</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s">
+        <v>15</v>
       </c>
       <c r="D86" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E86" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>14</v>
       </c>
+      <c r="B87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" t="s">
+        <v>16</v>
+      </c>
       <c r="D87" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E87" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30;TR1;TR2:30</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B88" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D88" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v>TR2:30PM3:45PM</v>
       </c>
       <c r="E88" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>TR2:30</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>6</v>
-      </c>
-      <c r="B89" t="s">
-        <v>4</v>
-      </c>
-      <c r="C89" t="s">
-        <v>32</v>
-      </c>
       <c r="D89" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF1:00PM2:10PM</v>
+        <v/>
       </c>
       <c r="E89" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF1-2:10</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D90" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>Trcheck10:30AM12:10PM</v>
-      </c>
-      <c r="E90" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>MWF1:00PM2:10PM</v>
+      </c>
+      <c r="E90" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF1-2:10</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D91" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>Mwcheck1:00PM2:15PM</v>
-      </c>
-      <c r="E91" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>MWF11:30AM12:40PM</v>
+      </c>
+      <c r="E91" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30-12:40</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>6</v>
+      </c>
+      <c r="B92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" t="s">
+        <v>31</v>
       </c>
       <c r="D92" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
+        <v>MWF11:30AM12:40PM</v>
       </c>
       <c r="E92" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>MWF11:30-12:40</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>14</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>15</v>
       </c>
       <c r="D93" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E93" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" t="s">
+        <v>19</v>
+      </c>
+      <c r="C94" t="s">
+        <v>31</v>
+      </c>
       <c r="D94" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF11:30AM12:40PM</v>
+      </c>
+      <c r="E94" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30-12:40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D95" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E94" t="str">
+      <c r="E95" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>14</v>
-      </c>
-      <c r="B95" t="s">
-        <v>4</v>
-      </c>
-      <c r="C95" t="s">
-        <v>16</v>
-      </c>
-      <c r="D95" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
-      </c>
-      <c r="E95" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>6</v>
-      </c>
-      <c r="B96" t="s">
-        <v>10</v>
-      </c>
-      <c r="C96" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="D96" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
-      </c>
-      <c r="E96" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>check</v>
+      </c>
+      <c r="E96" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B97" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D97" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E97" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B98" t="s">
         <v>4</v>
@@ -2494,88 +2506,97 @@
       </c>
       <c r="D98" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>MW1:00PM2:15PM</v>
       </c>
       <c r="E98" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MW1</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
       <c r="D99" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>F2:30PM4:00PM</v>
       </c>
       <c r="E99" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>F2:30-4:00</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B100" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C100" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D100" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E100" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B101" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C101" t="s">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="D101" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T6:00PM8:20PM</v>
-      </c>
-      <c r="E101" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>MWF11:30AM12:20PM</v>
+      </c>
+      <c r="E101" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s">
+        <v>15</v>
       </c>
       <c r="D102" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E102" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>4</v>
-      </c>
-      <c r="C103" t="s">
-        <v>5</v>
-      </c>
       <c r="D103" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E103" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2606,47 +2627,41 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>6</v>
-      </c>
-      <c r="B106" t="s">
-        <v>7</v>
-      </c>
-      <c r="C106" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D106" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM12:20PM</v>
+        <v>MWFno8</v>
       </c>
       <c r="E106" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30-12:20</v>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>4</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
       <c r="D107" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E107" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D108" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E107" t="str">
+      <c r="E108" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>4</v>
-      </c>
-      <c r="C108" t="s">
-        <v>5</v>
-      </c>
-      <c r="D108" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E108" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,45 +2681,48 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>6</v>
+      </c>
+      <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s">
+        <v>20</v>
+      </c>
       <c r="D110" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF10:30AM12:20PM</v>
+      </c>
+      <c r="E110" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF10:30-12:20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D111" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E110" t="str">
+      <c r="E111" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>6</v>
-      </c>
-      <c r="B111" t="s">
-        <v>17</v>
-      </c>
-      <c r="C111" t="s">
-        <v>18</v>
-      </c>
-      <c r="D111" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
-      </c>
-      <c r="E111" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
-      </c>
-    </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>110</v>
+      <c r="B112" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112" t="s">
+        <v>5</v>
       </c>
       <c r="D112" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFmorn</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E112" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -2718,51 +2736,55 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>4</v>
-      </c>
-      <c r="C114" t="s">
+      <c r="D114" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E114" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>4</v>
+      </c>
+      <c r="C115" t="s">
         <v>5</v>
       </c>
-      <c r="D114" t="str">
+      <c r="D115" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>1:00PM4:00PM</v>
       </c>
-      <c r="E114" t="str">
+      <c r="E115" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>14</v>
-      </c>
-      <c r="D115" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
-      </c>
-      <c r="E115" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>21</v>
-      </c>
-      <c r="B116" t="s">
-        <v>4</v>
-      </c>
-      <c r="C116" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D116" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM1:50PM</v>
+        <v>TR</v>
       </c>
       <c r="E116" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1</v>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" s="1" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF</v>
+      </c>
+      <c r="E117" s="1" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
   </sheetData>
@@ -2777,8 +2799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377702D3-3049-4D9F-8497-CBC60EF1DE1E}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3728,7 +3750,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="str">
+      <c r="A55" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWFmorn</v>
       </c>
@@ -3740,7 +3762,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="str">
+      <c r="A56" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TRmorn</v>
       </c>
@@ -3752,7 +3774,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="str">
+      <c r="A57" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>Trmorn</v>
       </c>
@@ -3764,7 +3786,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="str">
+      <c r="A58" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>morn</v>
       </c>
@@ -3776,7 +3798,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="str">
+      <c r="A59" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>no8morn</v>
       </c>
@@ -3788,7 +3810,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="str">
+      <c r="A60" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWFno8morn</v>
       </c>
@@ -3848,7 +3870,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="str">
+      <c r="A64" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>WR1:00PM4:00PM</v>
       </c>
@@ -3862,7 +3884,7 @@
         <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3884,7 +3906,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="str">
+      <c r="A66" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MTW1:00PM5:00PM</v>
       </c>
@@ -3898,7 +3920,7 @@
         <v>25</v>
       </c>
       <c r="E66" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update after finishing schedule for Spring 2025
Also completed feature to handle multiple cross-listed courses in one set
</commit_message>
<xml_diff>
--- a/Generate Time Codes.xlsx
+++ b/Generate Time Codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2024 Fall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2025 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71C9FAE9-8D5E-4453-9BBF-BC1B8084328E}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF01BC34-D789-4715-A509-3883DDBEC57F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>it has been 2:30-4:30 some semesters, but Mike said (2/13/2023) always make it 2:30-4:00</t>
         </r>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="128">
   <si>
     <t>days</t>
   </si>
@@ -438,7 +438,13 @@
     <t>M1-5;T1-5;W1-5</t>
   </si>
   <si>
-    <t>check</t>
+    <t>MWno8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MWF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MWF, either 10:30 or 11:30 </t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -481,21 +487,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -519,16 +517,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E117" totalsRowShown="0">
-  <autoFilter ref="A1:E117" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E101" totalsRowShown="0">
+  <autoFilter ref="A1:E101" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D6A4C193-C770-4795-BA4D-6659D41683A3}" name="days"/>
     <tableColumn id="2" xr3:uid="{E9079B6B-65A1-4117-9DF9-19A5E92BBBAE}" name="begin_time"/>
     <tableColumn id="3" xr3:uid="{91E2F62C-BC78-4486-8262-E8EB91EEAF07}" name="end_time"/>
-    <tableColumn id="4" xr3:uid="{F5DB56F5-5374-46A5-9F52-C165E95C7EB2}" name="merged_daytime" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{F5DB56F5-5374-46A5-9F52-C165E95C7EB2}" name="merged_daytime" dataDxfId="2">
       <calculatedColumnFormula>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{777DE3F8-1FE5-4C45-8E8A-95849F198C19}" name="timecode" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{777DE3F8-1FE5-4C45-8E8A-95849F198C19}" name="timecode" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -540,7 +538,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}" name="TimeCodeMap" displayName="TimeCodeMap" ref="A1:E67" totalsRowShown="0">
   <autoFilter ref="A1:E67" xr:uid="{B326F1B5-0A85-4DC6-B848-4E7E45CE36C0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3F488AE9-9DAA-41D9-8438-57EADAD189CE}" name="merged_daytime" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{3F488AE9-9DAA-41D9-8438-57EADAD189CE}" name="merged_daytime" dataDxfId="0">
       <calculatedColumnFormula>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{60CB15DE-0792-4C86-9DA9-F5946FF20273}" name="days"/>
@@ -553,9 +551,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -593,7 +591,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -699,7 +697,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -841,7 +839,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -849,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71782CAC-D457-4B7E-93F1-D92D90D65B94}">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E117"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,59 +880,50 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="D2" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW6:00PM7:30PM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E2" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW6-7:30</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
       <c r="D3" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R6:00PM9:00PM</v>
+        <v/>
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R6-9</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D4" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E4" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -977,7 +966,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -987,16 +976,16 @@
       </c>
       <c r="D7" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E7" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1006,118 +995,106 @@
       </c>
       <c r="D8" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E8" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
       <c r="D9" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E9" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D10" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E10" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
       </c>
       <c r="D11" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW8:00AM</v>
-      </c>
-      <c r="E11" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>MWF10:30AM11:20AM</v>
+      </c>
+      <c r="E11" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
       <c r="D12" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW2:30PM3:45PM</v>
+        <v/>
       </c>
       <c r="E12" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW2:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D13" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E13" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
       <c r="D14" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>MWF</v>
       </c>
       <c r="E14" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1127,49 +1104,49 @@
       </c>
       <c r="D15" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E15" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D16" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E16" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D17" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E17" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,18 +1154,18 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D18" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E18" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1196,61 +1173,61 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D19" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E19" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MWF8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D20" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E20" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D21" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E21" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
+        <v>T1-4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1260,54 +1237,45 @@
       </c>
       <c r="D22" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E22" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
+        <v>W1-4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="D23" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T9:30AM12:30PM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E23" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T9:30-12:30</v>
+        <v>R1-4</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
       <c r="D24" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E24" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
@@ -1317,187 +1285,169 @@
       </c>
       <c r="D25" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
-      </c>
-      <c r="E25" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
+        <v>F1:00PM4:00PM</v>
+      </c>
+      <c r="E25" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="D26" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R9:30AM12:30PM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E26" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R9:30-12:30</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
         <v>5</v>
       </c>
-      <c r="D27" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
-      </c>
-      <c r="E27" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>112</v>
-      </c>
       <c r="D28" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>morn</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E28" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
       <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>F1:00PM2:50PM</v>
+      </c>
+      <c r="E29" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>F1-2:50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E30" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF</v>
+      </c>
+      <c r="E31" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E33" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
         <v>5</v>
       </c>
-      <c r="D29" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E29" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM3:00PM</v>
-      </c>
-      <c r="E30" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E31" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
-      </c>
-      <c r="E32" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
-      </c>
-      <c r="E33" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D34" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E34" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>M1-4</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D35" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>check1:00PM4:00PM</v>
-      </c>
-      <c r="E35" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>MWF9:00AM9:50AM</v>
+      </c>
+      <c r="E35" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="D36" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM2:50PM</v>
-      </c>
-      <c r="E36" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1-2:50</v>
+        <v>MWno8</v>
+      </c>
+      <c r="E36" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,120 +1465,120 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D38" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E38" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
       <c r="D39" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E39" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D40" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>MWF8</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF</v>
+      </c>
+      <c r="E41" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E42" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E43" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
         <v>10</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C44" t="s">
         <v>11</v>
       </c>
-      <c r="D41" t="str">
+      <c r="D44" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>MWF9:00AM9:50AM</v>
       </c>
-      <c r="E41" t="str">
+      <c r="E44" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
-      </c>
-      <c r="E42" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:20AM</v>
-      </c>
-      <c r="E43" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E44" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1636,15 +1586,15 @@
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D45" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>1:00PM5:00PM</v>
       </c>
       <c r="E45" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1652,287 +1602,311 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM5:00PM</v>
+      </c>
+      <c r="E46" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" t="s">
         <v>5</v>
       </c>
-      <c r="D46" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E46" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D47" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>F2:30PM4:00PM</v>
       </c>
       <c r="E47" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>F2:30-4:00</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>F2:30PM4:00PM</v>
+      </c>
+      <c r="E48" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>F2:30-4:00</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>1:00PM4:00PM</v>
       </c>
-      <c r="E48" t="str">
+      <c r="E49" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D49" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E49" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" t="s">
-        <v>5</v>
+      <c r="A50" t="s">
+        <v>100</v>
       </c>
       <c r="D50" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>MWFno8</v>
       </c>
       <c r="E50" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D51" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E51" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D52" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>TR</v>
       </c>
       <c r="E52" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D53" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM5:00PM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E53" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5;W1-5;R1-5</v>
+        <v>MWF11:30</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" t="s">
-        <v>25</v>
+      <c r="A54" t="s">
+        <v>107</v>
       </c>
       <c r="D54" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM5:00PM</v>
+        <v>ASY</v>
       </c>
       <c r="E54" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5;W1-5;R1-5</v>
+        <v>ASY</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>8</v>
       </c>
       <c r="D55" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E55" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D56" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM5:00PM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E56" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>16</v>
+      </c>
       <c r="D57" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E57" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>127</v>
+      </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D58" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM5:00PM</v>
-      </c>
-      <c r="E58" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5;W1-5;R1-5</v>
+        <v>MWF, either 10:30 or 11:30 10:30AM11:20AM</v>
+      </c>
+      <c r="E58" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D59" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:00PM</v>
-      </c>
-      <c r="E59" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F2:30-4:00</v>
+        <v>MW11:30AM12:40PM</v>
+      </c>
+      <c r="E59" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>21</v>
-      </c>
-      <c r="B60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D60" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:00PM</v>
+        <v>MWF</v>
       </c>
       <c r="E60" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F2:30-4:00</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
       <c r="D61" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR</v>
+      </c>
+      <c r="E61" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D62" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E61" t="str">
+      <c r="E62" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
-      </c>
-      <c r="E62" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>24</v>
+      </c>
+      <c r="B63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" t="s">
+        <v>28</v>
       </c>
       <c r="D63" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>ASY</v>
+        <v>MW2:30PM3:45PM</v>
       </c>
       <c r="E63" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>ASY</v>
+        <v>MW2:30</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D64" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:20AM</v>
+        <v>MW11:30AM12:40PM</v>
       </c>
       <c r="E64" t="e">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
@@ -1940,73 +1914,61 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>6</v>
-      </c>
-      <c r="B65" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" t="s">
-        <v>11</v>
-      </c>
       <c r="D65" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v/>
       </c>
       <c r="E65" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B66" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" t="s">
-        <v>16</v>
-      </c>
       <c r="D66" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v/>
       </c>
       <c r="E66" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D67" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E67" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>125</v>
+        <v>14</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>15</v>
       </c>
       <c r="D68" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>check</v>
-      </c>
-      <c r="E68" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>TR10:30AM11:45AM</v>
+      </c>
+      <c r="E68" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2014,69 +1976,75 @@
         <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D69" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E69" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
       </c>
       <c r="D70" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>check</v>
-      </c>
-      <c r="E70" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>MWF10:30AM11:20AM</v>
+      </c>
+      <c r="E70" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF10:30</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B71" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D71" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MW1:00PM2:15PM</v>
       </c>
       <c r="E71" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>MW1</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D72" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M2:30PM4:30PM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E72" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M2:30-4:30</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2103,107 +2071,101 @@
         <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D74" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E74" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>107</v>
-      </c>
       <c r="D75" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>ASY</v>
+        <v/>
       </c>
       <c r="E75" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>ASY</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>14</v>
-      </c>
-      <c r="B76">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="C76">
-        <v>0.65625</v>
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" t="s">
+        <v>31</v>
       </c>
       <c r="D76" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR0.6041666666666670.65625</v>
-      </c>
-      <c r="E76" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>MWF11:30AM12:40PM</v>
+      </c>
+      <c r="E76" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30-12:40</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77" t="s">
-        <v>16</v>
-      </c>
       <c r="D77" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v/>
       </c>
       <c r="E77" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>24</v>
-      </c>
-      <c r="B78" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78" t="s">
-        <v>28</v>
-      </c>
       <c r="D78" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW2:30PM3:45PM</v>
+        <v/>
       </c>
       <c r="E78" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW2:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" t="s">
+        <v>31</v>
+      </c>
       <c r="D79" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>MWF11:30AM12:40PM</v>
       </c>
       <c r="E79" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>MWF11:30-12:40</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="B80" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" t="s">
+        <v>31</v>
       </c>
       <c r="D80" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>check</v>
+        <v>MWF 11:30AM12:40PM</v>
       </c>
       <c r="E80" t="e">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
@@ -2211,69 +2173,66 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>125</v>
-      </c>
       <c r="D81" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>check</v>
-      </c>
-      <c r="E81" t="e">
+        <v/>
+      </c>
+      <c r="E81" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" t="s">
+        <v>31</v>
+      </c>
+      <c r="D82" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MW11:30AM12:40PM</v>
+      </c>
+      <c r="E82" t="e">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>#N/A</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D82" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E82" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D83" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>TR10:30AM12:10PM</v>
       </c>
       <c r="E83" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
+        <v>TR10:30-12:10</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>6</v>
-      </c>
-      <c r="B84" t="s">
-        <v>7</v>
-      </c>
-      <c r="C84" t="s">
-        <v>8</v>
-      </c>
       <c r="D84" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v/>
       </c>
       <c r="E84" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B85" t="s">
         <v>4</v>
@@ -2283,508 +2242,267 @@
       </c>
       <c r="D85" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E85" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>TR1</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D86" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>MW2:30PM3:45PM</v>
       </c>
       <c r="E86" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MW2:30</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D87" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E87" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>MWF9</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF10:30AM11:20AM</v>
+      </c>
+      <c r="E88" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF10:30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>14</v>
       </c>
-      <c r="B88" t="s">
-        <v>26</v>
-      </c>
-      <c r="C88" t="s">
-        <v>28</v>
-      </c>
-      <c r="D88" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
-      </c>
-      <c r="E88" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s">
+        <v>15</v>
+      </c>
       <c r="D89" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E89" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>TR10:30</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C90" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D90" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF1:00PM2:10PM</v>
+        <v>TR2:30PM3:45PM</v>
       </c>
       <c r="E90" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF1-2:10</v>
+        <v>TR2:30</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>6</v>
-      </c>
-      <c r="B91" t="s">
-        <v>19</v>
-      </c>
-      <c r="C91" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="D91" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v>no8</v>
       </c>
       <c r="E91" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>6</v>
-      </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="D92" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E92" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>14</v>
-      </c>
-      <c r="B93" t="s">
-        <v>7</v>
-      </c>
-      <c r="C93" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="D93" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>no8</v>
       </c>
       <c r="E93" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>6</v>
-      </c>
       <c r="B94" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="D94" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E94" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
       <c r="D95" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>MWF</v>
       </c>
       <c r="E95" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>125</v>
+      <c r="B96" t="s">
+        <v>4</v>
+      </c>
+      <c r="C96" t="s">
+        <v>5</v>
       </c>
       <c r="D96" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>check</v>
-      </c>
-      <c r="E96" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E96" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>14</v>
-      </c>
       <c r="B97" t="s">
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D97" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E97" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>24</v>
-      </c>
-      <c r="B98" t="s">
-        <v>4</v>
-      </c>
-      <c r="C98" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="D98" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v>no8</v>
       </c>
       <c r="E98" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>21</v>
-      </c>
-      <c r="B99" t="s">
-        <v>26</v>
-      </c>
-      <c r="C99" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D99" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F2:30PM4:00PM</v>
+        <v>MWF</v>
       </c>
       <c r="E99" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F2:30-4:00</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>6</v>
       </c>
-      <c r="B100" t="s">
-        <v>7</v>
-      </c>
-      <c r="C100" t="s">
-        <v>8</v>
-      </c>
       <c r="D100" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>MWF</v>
       </c>
       <c r="E100" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B101" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C101" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D101" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>F1:00PM1:50PM</v>
       </c>
       <c r="E101" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>14</v>
-      </c>
-      <c r="B102" t="s">
-        <v>7</v>
-      </c>
-      <c r="C102" t="s">
-        <v>15</v>
-      </c>
-      <c r="D102" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E102" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D103" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E103" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D104" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E104" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>4</v>
-      </c>
-      <c r="C105" t="s">
-        <v>5</v>
-      </c>
-      <c r="D105" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E105" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>100</v>
-      </c>
-      <c r="D106" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
-      </c>
-      <c r="E106" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>4</v>
-      </c>
-      <c r="C107" t="s">
-        <v>5</v>
-      </c>
-      <c r="D107" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E107" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D108" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E108" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>4</v>
-      </c>
-      <c r="C109" t="s">
-        <v>5</v>
-      </c>
-      <c r="D109" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E109" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>6</v>
-      </c>
-      <c r="B110" t="s">
-        <v>7</v>
-      </c>
-      <c r="C110" t="s">
-        <v>20</v>
-      </c>
-      <c r="D110" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM12:20PM</v>
-      </c>
-      <c r="E110" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30-12:20</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D111" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E111" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
-        <v>4</v>
-      </c>
-      <c r="C112" t="s">
-        <v>5</v>
-      </c>
-      <c r="D112" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E112" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D113" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E113" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D114" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E114" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>4</v>
-      </c>
-      <c r="C115" t="s">
-        <v>5</v>
-      </c>
-      <c r="D115" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E115" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>14</v>
-      </c>
-      <c r="D116" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
-      </c>
-      <c r="E116" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" s="1" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
-      </c>
-      <c r="E117" s="1" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+        <v>F1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update after finishing schedule for Fall 2025
</commit_message>
<xml_diff>
--- a/Generate Time Codes.xlsx
+++ b/Generate Time Codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2025 Spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2025 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF01BC34-D789-4715-A509-3883DDBEC57F}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0C5D0A2-949E-4C97-A57A-29D9FDC42DB0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="126">
   <si>
     <t>days</t>
   </si>
@@ -438,13 +438,7 @@
     <t>M1-5;T1-5;W1-5</t>
   </si>
   <si>
-    <t>MWno8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MWF </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MWF, either 10:30 or 11:30 </t>
+    <t>MWf</t>
   </si>
 </sst>
 </file>
@@ -849,19 +843,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71782CAC-D457-4B7E-93F1-D92D90D65B94}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.265625" customWidth="1"/>
+    <col min="2" max="3" width="13.73046875" customWidth="1"/>
     <col min="4" max="4" width="24" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -878,55 +872,58 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF</v>
+      </c>
+      <c r="E2" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
-      </c>
-      <c r="E2" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>T1-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D4" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E4" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -945,26 +942,26 @@
         <v>MWF10:30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D6" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E6" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>M1-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -983,7 +980,7 @@
         <v>W1-4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +999,7 @@
         <v>R1-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D9" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
@@ -1012,55 +1009,46 @@
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D10" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v/>
       </c>
       <c r="E10" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D11" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v/>
       </c>
       <c r="E11" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
       <c r="D12" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E12" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>T1-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1079,39 +1067,45 @@
         <v>W1-4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>R1:00PM4:00PM</v>
+      </c>
+      <c r="E14" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>R1-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
-      </c>
-      <c r="E14" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D15" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E15" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1130,7 +1124,7 @@
         <v>MWF9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1149,7 +1143,7 @@
         <v>MWF10:30</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1168,45 +1162,45 @@
         <v>MWF11:30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D19" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E19" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>M1-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="D20" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>T9:30AM12:30PM</v>
       </c>
       <c r="E20" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>T9:30-12:30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1225,7 +1219,7 @@
         <v>T1-4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1244,55 +1238,55 @@
         <v>W1-4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>R9:30AM12:30PM</v>
+      </c>
+      <c r="E23" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>R9:30-12:30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
         <v>5</v>
       </c>
-      <c r="D23" t="str">
+      <c r="D24" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>R1:00PM4:00PM</v>
       </c>
-      <c r="E23" t="str">
+      <c r="E24" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>R1-4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D24" t="str">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D25" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E24" t="str">
+      <c r="E25" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM4:00PM</v>
-      </c>
-      <c r="E25" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1311,17 +1305,26 @@
         <v>M1-4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
       <c r="D27" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>F1:00PM3:00PM</v>
       </c>
       <c r="E27" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>F1-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>4</v>
       </c>
@@ -1337,26 +1340,20 @@
         <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D29" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM2:50PM</v>
+        <v>TR</v>
       </c>
       <c r="E29" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1-2:50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D30" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
@@ -1366,20 +1363,23 @@
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>6</v>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
       </c>
       <c r="D31" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E31" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D32" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
@@ -1389,164 +1389,188 @@
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
       <c r="D33" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR8:00AM9:15AM</v>
+      </c>
+      <c r="E33" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D34" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E33" t="str">
+      <c r="E34" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
-      </c>
-      <c r="E34" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>6</v>
       </c>
       <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF11:30AM12:20PM</v>
+      </c>
+      <c r="E35" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR8:00AM9:15AM</v>
+      </c>
+      <c r="E36" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>M1:00PM4:00PM</v>
+      </c>
+      <c r="E37" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>R1:00PM4:00PM</v>
+      </c>
+      <c r="E38" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>R1-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
         <v>10</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C39" t="s">
         <v>11</v>
       </c>
-      <c r="D35" t="str">
+      <c r="D39" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>MWF9:00AM9:50AM</v>
       </c>
-      <c r="E35" t="str">
+      <c r="E39" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D36" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWno8</v>
-      </c>
-      <c r="E36" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D37" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E37" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
-      </c>
-      <c r="E38" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E39" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>6</v>
-      </c>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D40" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E40" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>6</v>
       </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
       <c r="D41" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E41" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>125</v>
+      </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D42" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>MWf10:30AM11:20AM</v>
       </c>
       <c r="E42" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF10:30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
@@ -1555,49 +1579,55 @@
       </c>
       <c r="D43" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E43" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>T1-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>R1:00PM4:00PM</v>
+      </c>
+      <c r="E44" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>R1-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>6</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>10</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>11</v>
       </c>
-      <c r="D44" t="str">
+      <c r="D45" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>MWF9:00AM9:50AM</v>
       </c>
-      <c r="E44" t="str">
+      <c r="E45" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM5:00PM</v>
-      </c>
-      <c r="E45" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5;T1-5;W1-5;R1-5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
@@ -1606,486 +1636,441 @@
       </c>
       <c r="D46" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>M1:00PM5:00PM</v>
+      </c>
+      <c r="E46" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>T1:00PM5:00PM</v>
+      </c>
+      <c r="E47" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>T1-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR</v>
+      </c>
+      <c r="E48" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF</v>
+      </c>
+      <c r="E49" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>1:00PM5:00PM</v>
       </c>
-      <c r="E46" t="str">
+      <c r="E50" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>M1-5;T1-5;W1-5;R1-5</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>21</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B51" t="s">
         <v>26</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C51" t="s">
         <v>5</v>
       </c>
-      <c r="D47" t="str">
+      <c r="D51" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>F2:30PM4:00PM</v>
       </c>
-      <c r="E47" t="str">
+      <c r="E51" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>F2:30-4:00</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>21</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B52" t="s">
         <v>26</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C52" t="s">
         <v>5</v>
       </c>
-      <c r="D48" t="str">
+      <c r="D52" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>F2:30PM4:00PM</v>
       </c>
-      <c r="E48" t="str">
+      <c r="E52" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>F2:30-4:00</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E49" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
-      </c>
-      <c r="E50" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D53" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E53" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D54" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E54" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D55" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E55" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>6</v>
-      </c>
-      <c r="B51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
-      </c>
-      <c r="E51" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
-      </c>
-      <c r="E52" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
-      </c>
-      <c r="E53" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>107</v>
-      </c>
-      <c r="D54" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>ASY</v>
-      </c>
-      <c r="E54" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>ASY</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
-      </c>
-      <c r="E55" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>14</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D56" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E56" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" t="s">
+        <v>MWF10:30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D57" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E57" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF11:30AM12:20PM</v>
+      </c>
+      <c r="E58" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D59" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E59" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>M2:30PM4:30PM</v>
+      </c>
+      <c r="E60" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M2:30-4:30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
         <v>16</v>
       </c>
-      <c r="D57" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
-      </c>
-      <c r="E57" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B58" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF, either 10:30 or 11:30 10:30AM11:20AM</v>
-      </c>
-      <c r="E58" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59" t="s">
-        <v>19</v>
-      </c>
-      <c r="C59" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW11:30AM12:40PM</v>
-      </c>
-      <c r="E59" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="D61" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MW1:00PM2:15PM</v>
+      </c>
+      <c r="E61" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MW1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D62" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E62" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D63" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E63" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D64" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E64" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>T8:00AM8:50AM</v>
+      </c>
+      <c r="E65" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>T8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>W2:30PM3:20PM</v>
+      </c>
+      <c r="E66" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>W2:30-3:20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D67" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E67" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>6</v>
       </c>
-      <c r="D60" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
-      </c>
-      <c r="E60" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
-      </c>
-      <c r="E61" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D62" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E62" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" t="s">
-        <v>26</v>
-      </c>
-      <c r="C63" t="s">
-        <v>28</v>
-      </c>
-      <c r="D63" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW2:30PM3:45PM</v>
-      </c>
-      <c r="E63" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW2:30</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>24</v>
-      </c>
-      <c r="B64" t="s">
-        <v>19</v>
-      </c>
-      <c r="C64" t="s">
-        <v>31</v>
-      </c>
-      <c r="D64" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW11:30AM12:40PM</v>
-      </c>
-      <c r="E64" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D65" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E65" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D66" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E66" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>10</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>11</v>
       </c>
-      <c r="D67" t="str">
+      <c r="D68" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>MWF9:00AM9:50AM</v>
       </c>
-      <c r="E67" t="str">
+      <c r="E68" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF9</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>14</v>
-      </c>
-      <c r="B68" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E68" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D69" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E69" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF10:30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MW1:00PM2:15PM</v>
+      </c>
+      <c r="E70" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MW1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" t="s">
         <v>7</v>
       </c>
-      <c r="C70" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
-      </c>
-      <c r="E70" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B71" t="s">
-        <v>4</v>
-      </c>
       <c r="C71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D71" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E71" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>TR10:30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D72" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E72" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>TR1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C73" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D73" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
+        <v>TR2:30PM3:45PM</v>
       </c>
       <c r="E73" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s">
-        <v>15</v>
-      </c>
+        <v>TR2:30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D74" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
+        <v/>
       </c>
       <c r="E74" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D75" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
@@ -2095,7 +2080,7 @@
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2114,48 +2099,66 @@
         <v>MWF11:30-12:40</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>33</v>
+      </c>
       <c r="D77" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>TR10:30AM12:10PM</v>
       </c>
       <c r="E77" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>TR10:30-12:10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" t="s">
+        <v>31</v>
+      </c>
       <c r="D78" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>MWF11:30AM12:40PM</v>
       </c>
       <c r="E78" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF11:30-12:40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR10:30AM11:45AM</v>
+      </c>
+      <c r="E79" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR10:30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
         <v>6</v>
-      </c>
-      <c r="B79" t="s">
-        <v>19</v>
-      </c>
-      <c r="C79" t="s">
-        <v>31</v>
-      </c>
-      <c r="D79" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
-      </c>
-      <c r="E79" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>126</v>
       </c>
       <c r="B80" t="s">
         <v>19</v>
@@ -2165,14 +2168,14 @@
       </c>
       <c r="D80" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF 11:30AM12:40PM</v>
-      </c>
-      <c r="E80" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF11:30AM12:40PM</v>
+      </c>
+      <c r="E80" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30-12:40</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D81" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
@@ -2182,272 +2185,239 @@
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D82" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW11:30AM12:40PM</v>
-      </c>
-      <c r="E82" t="e">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>14</v>
-      </c>
-      <c r="B83" t="s">
+        <v>TR1:00PM2:15PM</v>
+      </c>
+      <c r="E82" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D83" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E83" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D84" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E84" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D85" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E85" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" t="s">
         <v>7</v>
       </c>
-      <c r="C83" t="s">
-        <v>33</v>
-      </c>
-      <c r="D83" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM12:10PM</v>
-      </c>
-      <c r="E83" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30-12:10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D84" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E84" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>14</v>
-      </c>
-      <c r="B85" t="s">
-        <v>4</v>
-      </c>
-      <c r="C85" t="s">
-        <v>16</v>
-      </c>
-      <c r="D85" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
-      </c>
-      <c r="E85" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>24</v>
-      </c>
-      <c r="B86" t="s">
-        <v>26</v>
-      </c>
       <c r="C86" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D86" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW2:30PM3:45PM</v>
+        <v>MWF10:30AM11:20AM</v>
       </c>
       <c r="E86" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW2:30</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF10:30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C87" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D87" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E87" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF11:30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR1:00PM2:15PM</v>
+      </c>
+      <c r="E88" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D89" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E89" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D90" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWFno8</v>
+      </c>
+      <c r="E90" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E91" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>98</v>
+      </c>
+      <c r="D92" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>no8</v>
+      </c>
+      <c r="E92" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B93" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E93" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR</v>
+      </c>
+      <c r="E94" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B95" t="s">
+        <v>4</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E95" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
         <v>6</v>
       </c>
-      <c r="B88" t="s">
-        <v>7</v>
-      </c>
-      <c r="C88" t="s">
-        <v>8</v>
-      </c>
-      <c r="D88" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
-      </c>
-      <c r="E88" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>14</v>
-      </c>
-      <c r="B89" t="s">
-        <v>7</v>
-      </c>
-      <c r="C89" t="s">
-        <v>15</v>
-      </c>
-      <c r="D89" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E89" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>14</v>
-      </c>
-      <c r="B90" t="s">
-        <v>26</v>
-      </c>
-      <c r="C90" t="s">
-        <v>28</v>
-      </c>
-      <c r="D90" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
-      </c>
-      <c r="E90" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>98</v>
-      </c>
-      <c r="D91" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
-      </c>
-      <c r="E91" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>4</v>
-      </c>
-      <c r="C92" t="s">
-        <v>5</v>
-      </c>
-      <c r="D92" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E92" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>98</v>
-      </c>
-      <c r="D93" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
-      </c>
-      <c r="E93" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>4</v>
-      </c>
-      <c r="C94" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E94" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>6</v>
-      </c>
-      <c r="D95" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
-      </c>
-      <c r="E95" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C96" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D96" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E96" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>4</v>
-      </c>
-      <c r="C97" t="s">
-        <v>5</v>
-      </c>
+        <v>MWF11:30</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D97" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E97" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -2460,20 +2430,23 @@
         <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>6</v>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B99" t="s">
+        <v>4</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
       </c>
       <c r="D99" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E99" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -2486,23 +2459,17 @@
         <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>21</v>
-      </c>
-      <c r="B101" t="s">
-        <v>4</v>
-      </c>
-      <c r="C101" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="D101" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM1:50PM</v>
+        <v>no8</v>
       </c>
       <c r="E101" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1</v>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
   </sheetData>
@@ -2517,19 +2484,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377702D3-3049-4D9F-8497-CBC60EF1DE1E}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1328125" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" customWidth="1"/>
+    <col min="3" max="4" width="14.1328125" customWidth="1"/>
+    <col min="5" max="5" width="29.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -2546,7 +2513,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF8:00AM8:50AM</v>
@@ -2564,7 +2531,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF9:00AM9:50AM</v>
@@ -2582,7 +2549,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF10:30AM11:20AM</v>
@@ -2600,7 +2567,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF11:30AM12:20PM</v>
@@ -2618,7 +2585,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW8:00AM8:50AM</v>
@@ -2636,7 +2603,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW9:00AM9:50AM</v>
@@ -2654,7 +2621,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW10:30AM11:20AM</v>
@@ -2672,7 +2639,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW11:30AM12:20PM</v>
@@ -2690,7 +2657,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF1:00PM1:50PM</v>
@@ -2708,7 +2675,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF2:30PM3:20PM</v>
@@ -2726,7 +2693,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW1:00PM2:15PM</v>
@@ -2744,7 +2711,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW2:30PM3:45PM</v>
@@ -2762,7 +2729,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW4:00PM5:15PM</v>
@@ -2780,7 +2747,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>M1:00PM4:00PM</v>
@@ -2798,7 +2765,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>M1:00PM5:00PM</v>
@@ -2816,7 +2783,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>W1:00PM4:00PM</v>
@@ -2834,7 +2801,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>W1:00PM5:00PM</v>
@@ -2852,7 +2819,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR8:00AM9:15AM</v>
@@ -2870,7 +2837,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR10:30AM11:45AM</v>
@@ -2888,7 +2855,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR1:00PM2:15PM</v>
@@ -2906,7 +2873,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR2:30PM3:45PM</v>
@@ -2924,7 +2891,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T1:00PM4:00PM</v>
@@ -2942,7 +2909,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T1:00PM5:00PM</v>
@@ -2960,7 +2927,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R1:00PM4:00PM</v>
@@ -2978,7 +2945,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R1:00PM5:00PM</v>
@@ -2996,7 +2963,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF11:30AM12:40PM</v>
@@ -3014,7 +2981,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF1:00PM2:10PM</v>
@@ -3032,7 +2999,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR10:30AM12:10PM</v>
@@ -3050,7 +3017,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF10:30AM12:20PM</v>
@@ -3068,7 +3035,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>M6:00PM9:00PM</v>
@@ -3086,7 +3053,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T6:00PM9:00PM</v>
@@ -3104,7 +3071,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R6:00PM9:00PM</v>
@@ -3122,7 +3089,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR6:00PM7:15PM</v>
@@ -3140,7 +3107,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T6:00PM8:30PM</v>
@@ -3158,7 +3125,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T9:30AM12:30PM</v>
@@ -3176,7 +3143,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R9:30AM12:30PM</v>
@@ -3194,7 +3161,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T8:00AM8:50AM</v>
@@ -3212,7 +3179,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R8:00AM8:50AM</v>
@@ -3230,7 +3197,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T2:30PM3:20PM</v>
@@ -3248,7 +3215,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>W2:30PM3:20PM</v>
@@ -3266,7 +3233,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW6:00PM7:30PM</v>
@@ -3284,7 +3251,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW11:30AM12:45PM</v>
@@ -3302,7 +3269,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F1:00PM1:50PM</v>
@@ -3320,7 +3287,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F1:00PM2:50PM</v>
@@ -3338,7 +3305,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F1:00PM3:00PM</v>
@@ -3356,7 +3323,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F1:30PM3:30PM</v>
@@ -3374,7 +3341,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F2:30PM4:00PM</v>
@@ -3392,7 +3359,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>M2:30PM4:30PM</v>
@@ -3410,7 +3377,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF</v>
@@ -3422,7 +3389,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR</v>
@@ -3434,7 +3401,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v/>
@@ -3443,7 +3410,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>no8</v>
@@ -3455,7 +3422,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWFno8</v>
@@ -3467,7 +3434,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWFmorn</v>
@@ -3479,7 +3446,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TRmorn</v>
@@ -3491,7 +3458,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>Trmorn</v>
@@ -3503,7 +3470,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>morn</v>
@@ -3515,7 +3482,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>no8morn</v>
@@ -3527,7 +3494,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWFno8morn</v>
@@ -3539,7 +3506,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>1:00PM4:00PM</v>
@@ -3554,7 +3521,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>1:00PM5:00PM</v>
@@ -3569,7 +3536,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TWR1:00PM4:00PM</v>
@@ -3587,7 +3554,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>WR1:00PM4:00PM</v>
@@ -3605,7 +3572,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MT1:00PM5:00PM</v>
@@ -3623,7 +3590,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MTW1:00PM5:00PM</v>
@@ -3641,7 +3608,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>ASY</v>

</xml_diff>

<commit_message>
Update after finishing schedule for Spring 2026
</commit_message>
<xml_diff>
--- a/Generate Time Codes.xlsx
+++ b/Generate Time Codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2025 Fall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2632d998cf74fae/Work/Physics/Course Scheduling Algorithm/2026 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0C5D0A2-949E-4C97-A57A-29D9FDC42DB0}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="8_{E073A633-F2D1-40E3-8B83-214455B05D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59611288-B5F1-40EE-80AD-629840BF0131}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
+    <workbookView minimized="1" xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{9DA971FE-66E9-40AE-8A0C-0B37A5B7993B}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="125">
   <si>
     <t>days</t>
   </si>
@@ -436,9 +436,6 @@
   </si>
   <si>
     <t>M1-5;T1-5;W1-5</t>
-  </si>
-  <si>
-    <t>MWf</t>
   </si>
 </sst>
 </file>
@@ -511,8 +508,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E101" totalsRowShown="0">
-  <autoFilter ref="A1:E101" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}" name="Table2" displayName="Table2" ref="A1:E96" totalsRowShown="0">
+  <autoFilter ref="A1:E96" xr:uid="{140717F8-C523-4918-92B1-722FA64C0A93}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D6A4C193-C770-4795-BA4D-6659D41683A3}" name="days"/>
     <tableColumn id="2" xr3:uid="{E9079B6B-65A1-4117-9DF9-19A5E92BBBAE}" name="begin_time"/>
@@ -841,21 +838,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71782CAC-D457-4B7E-93F1-D92D90D65B94}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.265625" customWidth="1"/>
-    <col min="2" max="3" width="13.73046875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="24" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -872,58 +869,55 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
       <c r="D2" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v>M1:00PM4:00PM</v>
       </c>
       <c r="E2" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
+        <v>M1-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="D4" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>R6:00PM9:00PM</v>
       </c>
       <c r="E4" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>R6-9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -942,28 +936,28 @@
         <v>MWF10:30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D6" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>MWF11:30AM12:20PM</v>
       </c>
       <c r="E6" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>MWF11:30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -973,16 +967,16 @@
       </c>
       <c r="D7" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W1:00PM4:00PM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E7" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W1-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>T1-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -992,14 +986,14 @@
       </c>
       <c r="D8" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>W1:00PM4:00PM</v>
       </c>
       <c r="E8" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>W1-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
@@ -1009,46 +1003,55 @@
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
       <c r="D10" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF9:00AM9:50AM</v>
+      </c>
+      <c r="E10" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF10:30AM11:20AM</v>
+      </c>
+      <c r="E11" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF10:30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E10" t="str">
+      <c r="E12" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D11" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E11" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
-      </c>
-      <c r="E12" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1067,140 +1070,134 @@
         <v>W1-4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF</v>
+      </c>
+      <c r="E14" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
-      </c>
-      <c r="E14" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
       <c r="D15" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
+        <v>T1:00PM4:00PM</v>
       </c>
       <c r="E15" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+        <v>T1-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D16" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v>MWF8:00AM8:50AM</v>
       </c>
       <c r="E16" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+        <v>MWF8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D17" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>MWF9:00AM9:50AM</v>
       </c>
       <c r="E17" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+        <v>MWF9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF10:30AM11:20AM</v>
+      </c>
+      <c r="E18" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF10:30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D19" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>MWF11:30AM12:20PM</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E19" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF11:30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
         <v>5</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D20" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>M1:00PM4:00PM</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E20" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>M1-4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T9:30AM12:30PM</v>
-      </c>
-      <c r="E20" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T9:30-12:30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1219,7 +1216,7 @@
         <v>T1-4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1238,55 +1235,58 @@
         <v>W1-4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="D23" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R9:30AM12:30PM</v>
+        <v>R1:00PM4:00PM</v>
       </c>
       <c r="E23" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R9:30-12:30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+        <v>R1-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D24" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>TR</v>
       </c>
       <c r="E24" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>90</v>
+      </c>
       <c r="D25" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
+        <v>F1:00PM3:00PM</v>
       </c>
       <c r="E25" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+        <v>F1-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1305,26 +1305,17 @@
         <v>M1-4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>90</v>
-      </c>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>F1:00PM3:00PM</v>
+        <v/>
       </c>
       <c r="E27" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>F1-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>4</v>
       </c>
@@ -1340,20 +1331,26 @@
         <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
       </c>
       <c r="D29" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
+        <v>F1:00PM2:50PM</v>
       </c>
       <c r="E29" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+        <v>F1-2:50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
@@ -1363,81 +1360,66 @@
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E31" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
         <v>5</v>
       </c>
-      <c r="D31" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E31" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D32" t="str">
+      <c r="D33" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>M1:00PM4:00PM</v>
+      </c>
+      <c r="E33" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E32" t="str">
+      <c r="E34" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR8:00AM9:15AM</v>
-      </c>
-      <c r="E33" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D34" t="str">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E34" t="str">
+      <c r="E35" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
-      </c>
-      <c r="E35" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1456,10 +1438,7 @@
         <v>TR8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>3</v>
-      </c>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>4</v>
       </c>
@@ -1468,52 +1447,34 @@
       </c>
       <c r="D37" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM4:00PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E37" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D38" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v/>
       </c>
       <c r="E38" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" t="s">
-        <v>11</v>
-      </c>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D39" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
+        <v/>
       </c>
       <c r="E39" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>4</v>
       </c>
@@ -1529,67 +1490,52 @@
         <v>M1-4;T1-4;W1-4;R1-4</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E41" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E42" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>6</v>
       </c>
-      <c r="B41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF8:00AM8:50AM</v>
-      </c>
-      <c r="E41" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>8</v>
       </c>
-      <c r="D42" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWf10:30AM11:20AM</v>
-      </c>
-      <c r="E42" t="str">
+      <c r="D43" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF10:30AM11:20AM</v>
+      </c>
+      <c r="E43" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF10:30</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM4:00PM</v>
-      </c>
-      <c r="E43" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>9</v>
-      </c>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>4</v>
       </c>
@@ -1598,55 +1544,49 @@
       </c>
       <c r="D44" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>R1:00PM4:00PM</v>
+        <v>1:00PM4:00PM</v>
       </c>
       <c r="E44" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>R1-4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E45" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>6</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>10</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>11</v>
       </c>
-      <c r="D45" t="str">
+      <c r="D46" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>MWF9:00AM9:50AM</v>
       </c>
-      <c r="E45" t="str">
+      <c r="E46" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M1:00PM5:00PM</v>
-      </c>
-      <c r="E46" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>12</v>
-      </c>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>4</v>
       </c>
@@ -1655,40 +1595,40 @@
       </c>
       <c r="D47" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T1:00PM5:00PM</v>
+        <v>1:00PM5:00PM</v>
       </c>
       <c r="E47" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T1-5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>14</v>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
       </c>
       <c r="D48" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR</v>
+        <v>1:00PM5:00PM</v>
       </c>
       <c r="E48" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR8;TR10:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>6</v>
-      </c>
+        <v>M1-5;T1-5;W1-5;R1-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D49" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
+        <v/>
       </c>
       <c r="E49" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>4</v>
       </c>
@@ -1704,7 +1644,7 @@
         <v>M1-5;T1-5;W1-5;R1-5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>21</v>
       </c>
@@ -1723,7 +1663,7 @@
         <v>F2:30-4:00</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>21</v>
       </c>
@@ -1742,251 +1682,275 @@
         <v>F2:30-4:00</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
       <c r="D53" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E53" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D54" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E53" t="str">
+      <c r="E54" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D54" t="str">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF11:30AM12:20PM</v>
+      </c>
+      <c r="E55" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>ASY</v>
+      </c>
+      <c r="E56" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>ASY</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR</v>
+      </c>
+      <c r="E57" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MW</v>
+      </c>
+      <c r="E58" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MW</v>
+      </c>
+      <c r="E59" t="e">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR</v>
+      </c>
+      <c r="E60" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR</v>
+      </c>
+      <c r="E61" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR8;TR10:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D62" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E54" t="str">
+      <c r="E62" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D55" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E55" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>W2:30PM3:20PM</v>
+      </c>
+      <c r="E63" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>W2:30-3:20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>6</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF9:00AM9:50AM</v>
+      </c>
+      <c r="E64" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
         <v>7</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR10:30AM11:45AM</v>
+      </c>
+      <c r="E65" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR10:30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF9:00AM9:50AM</v>
+      </c>
+      <c r="E66" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
         <v>8</v>
       </c>
-      <c r="D56" t="str">
+      <c r="D67" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>MWF10:30AM11:20AM</v>
       </c>
-      <c r="E56" t="str">
+      <c r="E67" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF10:30</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D57" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E57" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" t="s">
-        <v>19</v>
-      </c>
-      <c r="C58" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
-      </c>
-      <c r="E58" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D59" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E59" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>M2:30PM4:30PM</v>
-      </c>
-      <c r="E60" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M2:30-4:30</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>24</v>
       </c>
-      <c r="B61" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B68" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" t="s">
         <v>16</v>
       </c>
-      <c r="D61" t="str">
+      <c r="D68" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>MW1:00PM2:15PM</v>
       </c>
-      <c r="E61" t="str">
+      <c r="E68" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MW1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D62" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E62" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D63" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E63" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D64" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E64" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" t="s">
-        <v>18</v>
-      </c>
-      <c r="D65" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>T8:00AM8:50AM</v>
-      </c>
-      <c r="E65" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>T8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" t="s">
-        <v>26</v>
-      </c>
-      <c r="C66" t="s">
-        <v>29</v>
-      </c>
-      <c r="D66" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>W2:30PM3:20PM</v>
-      </c>
-      <c r="E66" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>W2:30-3:20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D67" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E67" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>6</v>
-      </c>
-      <c r="B68" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF9:00AM9:50AM</v>
-      </c>
-      <c r="E68" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D69" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>TR10:30AM11:45AM</v>
       </c>
       <c r="E69" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+        <v>TR10:30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B70" t="s">
         <v>4</v>
@@ -1996,480 +1960,394 @@
       </c>
       <c r="D70" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MW1:00PM2:15PM</v>
+        <v>TR1:00PM2:15PM</v>
       </c>
       <c r="E70" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MW1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+        <v>TR1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D71" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E71" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF11:30AM12:40PM</v>
+      </c>
+      <c r="E72" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30-12:40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D73" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E73" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D74" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E74" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" t="s">
+        <v>31</v>
+      </c>
+      <c r="D75" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF11:30AM12:40PM</v>
+      </c>
+      <c r="E75" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30-12:40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>14</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B76" t="s">
         <v>7</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C76" t="s">
         <v>15</v>
       </c>
-      <c r="D71" t="str">
+      <c r="D76" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>TR10:30AM11:45AM</v>
       </c>
-      <c r="E71" t="str">
+      <c r="E76" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>TR10:30</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D77" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E77" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D78" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E78" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" t="s">
+        <v>31</v>
+      </c>
+      <c r="D79" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF11:30AM12:40PM</v>
+      </c>
+      <c r="E79" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF11:30-12:40</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D80" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v/>
+      </c>
+      <c r="E80" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>14</v>
       </c>
-      <c r="B72" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" t="s">
         <v>16</v>
       </c>
-      <c r="D72" t="str">
+      <c r="D81" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>TR1:00PM2:15PM</v>
       </c>
-      <c r="E72" t="str">
+      <c r="E81" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>TR1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF9:00AM9:50AM</v>
+      </c>
+      <c r="E82" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF10:30AM11:20AM</v>
+      </c>
+      <c r="E83" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF10:30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>14</v>
       </c>
-      <c r="B73" t="s">
-        <v>26</v>
-      </c>
-      <c r="C73" t="s">
-        <v>28</v>
-      </c>
-      <c r="D73" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR2:30PM3:45PM</v>
-      </c>
-      <c r="E73" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR2:30</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D74" t="str">
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>TR10:30AM11:45AM</v>
+      </c>
+      <c r="E84" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>TR10:30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D85" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v/>
       </c>
-      <c r="E74" t="str">
+      <c r="E85" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D75" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E75" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>6</v>
-      </c>
-      <c r="B76" t="s">
-        <v>19</v>
-      </c>
-      <c r="C76" t="s">
-        <v>31</v>
-      </c>
-      <c r="D76" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
-      </c>
-      <c r="E76" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" t="s">
-        <v>33</v>
-      </c>
-      <c r="D77" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM12:10PM</v>
-      </c>
-      <c r="E77" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30-12:10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>6</v>
-      </c>
-      <c r="B78" t="s">
-        <v>19</v>
-      </c>
-      <c r="C78" t="s">
-        <v>31</v>
-      </c>
-      <c r="D78" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
-      </c>
-      <c r="E78" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>14</v>
-      </c>
-      <c r="B79" t="s">
-        <v>7</v>
-      </c>
-      <c r="C79" t="s">
-        <v>15</v>
-      </c>
-      <c r="D79" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR10:30AM11:45AM</v>
-      </c>
-      <c r="E79" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR10:30</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>6</v>
-      </c>
-      <c r="B80" t="s">
-        <v>19</v>
-      </c>
-      <c r="C80" t="s">
-        <v>31</v>
-      </c>
-      <c r="D80" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:40PM</v>
-      </c>
-      <c r="E80" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30-12:40</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D81" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E81" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>14</v>
-      </c>
-      <c r="B82" t="s">
-        <v>4</v>
-      </c>
-      <c r="C82" t="s">
-        <v>16</v>
-      </c>
-      <c r="D82" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
-      </c>
-      <c r="E82" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D83" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E83" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D84" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E84" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D85" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E85" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>6</v>
       </c>
-      <c r="B86" t="s">
-        <v>7</v>
-      </c>
-      <c r="C86" t="s">
-        <v>8</v>
-      </c>
       <c r="D86" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF10:30AM11:20AM</v>
+        <v>MWF</v>
       </c>
       <c r="E86" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF10:30</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E87" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>6</v>
       </c>
-      <c r="B87" t="s">
-        <v>19</v>
-      </c>
-      <c r="C87" t="s">
-        <v>20</v>
-      </c>
-      <c r="D87" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
-      </c>
-      <c r="E87" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
+      <c r="D88" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF</v>
+      </c>
+      <c r="E88" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E89" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E90" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>98</v>
+      </c>
+      <c r="D91" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>no8</v>
+      </c>
+      <c r="E91" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>MWF</v>
+      </c>
+      <c r="E92" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>98</v>
+      </c>
+      <c r="D93" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>no8</v>
+      </c>
+      <c r="E93" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" t="str">
+        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
+        <v>1:00PM4:00PM</v>
+      </c>
+      <c r="E94" t="str">
+        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
+        <v>M1-4;T1-4;W1-4;R1-4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>14</v>
       </c>
-      <c r="B88" t="s">
-        <v>4</v>
-      </c>
-      <c r="C88" t="s">
-        <v>16</v>
-      </c>
-      <c r="D88" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>TR1:00PM2:15PM</v>
-      </c>
-      <c r="E88" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>TR1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D89" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E89" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A90" t="s">
-        <v>100</v>
-      </c>
-      <c r="D90" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWFno8</v>
-      </c>
-      <c r="E90" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B91" t="s">
-        <v>4</v>
-      </c>
-      <c r="C91" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E91" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A92" t="s">
-        <v>98</v>
-      </c>
-      <c r="D92" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
-      </c>
-      <c r="E92" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B93" t="s">
-        <v>4</v>
-      </c>
-      <c r="C93" t="s">
-        <v>5</v>
-      </c>
-      <c r="D93" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E93" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A94" t="s">
-        <v>14</v>
-      </c>
-      <c r="D94" t="str">
+      <c r="D95" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
         <v>TR</v>
       </c>
-      <c r="E94" t="str">
+      <c r="E95" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
         <v>TR8;TR10:30;TR1;TR2:30</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B95" t="s">
-        <v>4</v>
-      </c>
-      <c r="C95" t="s">
-        <v>5</v>
-      </c>
-      <c r="D95" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E95" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B96" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D96" t="str">
         <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF11:30AM12:20PM</v>
+        <v>F1:00PM1:50PM</v>
       </c>
       <c r="E96" t="str">
         <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF11:30</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D97" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v/>
-      </c>
-      <c r="E97" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;TR8;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A98" t="s">
-        <v>98</v>
-      </c>
-      <c r="D98" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
-      </c>
-      <c r="E98" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B99" t="s">
-        <v>4</v>
-      </c>
-      <c r="C99" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>1:00PM4:00PM</v>
-      </c>
-      <c r="E99" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>M1-4;T1-4;W1-4;R1-4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A100" t="s">
-        <v>6</v>
-      </c>
-      <c r="D100" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>MWF</v>
-      </c>
-      <c r="E100" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF8;MWF9;MWF10:30;MWF11:30;MW1;MW2:30</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
-        <v>98</v>
-      </c>
-      <c r="D101" t="str">
-        <f>Table2[[#This Row],[days]]&amp;Table2[[#This Row],[begin_time]]&amp;Table2[[#This Row],[end_time]]</f>
-        <v>no8</v>
-      </c>
-      <c r="E101" t="str">
-        <f>VLOOKUP(Table2[[#This Row],[merged_daytime]],TimeCodeMap[],5,FALSE)</f>
-        <v>MWF9;MWF10:30;MWF11:30;TR10:30;MW1;MW2:30;TR1;TR2:30</v>
+        <v>F1</v>
       </c>
     </row>
   </sheetData>
@@ -2484,19 +2362,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377702D3-3049-4D9F-8497-CBC60EF1DE1E}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1328125" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" customWidth="1"/>
-    <col min="3" max="4" width="14.1328125" customWidth="1"/>
-    <col min="5" max="5" width="29.86328125" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -2513,7 +2391,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF8:00AM8:50AM</v>
@@ -2531,7 +2409,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF9:00AM9:50AM</v>
@@ -2549,7 +2427,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF10:30AM11:20AM</v>
@@ -2567,7 +2445,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF11:30AM12:20PM</v>
@@ -2585,7 +2463,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW8:00AM8:50AM</v>
@@ -2603,7 +2481,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW9:00AM9:50AM</v>
@@ -2621,7 +2499,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW10:30AM11:20AM</v>
@@ -2639,7 +2517,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW11:30AM12:20PM</v>
@@ -2657,7 +2535,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF1:00PM1:50PM</v>
@@ -2675,7 +2553,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF2:30PM3:20PM</v>
@@ -2693,7 +2571,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW1:00PM2:15PM</v>
@@ -2711,7 +2589,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW2:30PM3:45PM</v>
@@ -2729,7 +2607,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW4:00PM5:15PM</v>
@@ -2747,7 +2625,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>M1:00PM4:00PM</v>
@@ -2765,7 +2643,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>M1:00PM5:00PM</v>
@@ -2783,7 +2661,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>W1:00PM4:00PM</v>
@@ -2801,7 +2679,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>W1:00PM5:00PM</v>
@@ -2819,7 +2697,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR8:00AM9:15AM</v>
@@ -2837,7 +2715,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR10:30AM11:45AM</v>
@@ -2855,7 +2733,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR1:00PM2:15PM</v>
@@ -2873,7 +2751,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR2:30PM3:45PM</v>
@@ -2891,7 +2769,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T1:00PM4:00PM</v>
@@ -2909,7 +2787,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T1:00PM5:00PM</v>
@@ -2927,7 +2805,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R1:00PM4:00PM</v>
@@ -2945,7 +2823,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R1:00PM5:00PM</v>
@@ -2963,7 +2841,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF11:30AM12:40PM</v>
@@ -2981,7 +2859,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF1:00PM2:10PM</v>
@@ -2999,7 +2877,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR10:30AM12:10PM</v>
@@ -3017,7 +2895,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF10:30AM12:20PM</v>
@@ -3035,7 +2913,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>M6:00PM9:00PM</v>
@@ -3053,7 +2931,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T6:00PM9:00PM</v>
@@ -3071,7 +2949,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R6:00PM9:00PM</v>
@@ -3089,7 +2967,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR6:00PM7:15PM</v>
@@ -3107,7 +2985,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T6:00PM8:30PM</v>
@@ -3125,7 +3003,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T9:30AM12:30PM</v>
@@ -3143,7 +3021,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R9:30AM12:30PM</v>
@@ -3161,7 +3039,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T8:00AM8:50AM</v>
@@ -3179,7 +3057,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>R8:00AM8:50AM</v>
@@ -3197,7 +3075,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>T2:30PM3:20PM</v>
@@ -3215,7 +3093,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>W2:30PM3:20PM</v>
@@ -3233,7 +3111,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW6:00PM7:30PM</v>
@@ -3251,7 +3129,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MW11:30AM12:45PM</v>
@@ -3269,7 +3147,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F1:00PM1:50PM</v>
@@ -3287,7 +3165,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F1:00PM2:50PM</v>
@@ -3305,7 +3183,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F1:00PM3:00PM</v>
@@ -3323,7 +3201,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F1:30PM3:30PM</v>
@@ -3341,7 +3219,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>F2:30PM4:00PM</v>
@@ -3359,7 +3237,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>M2:30PM4:30PM</v>
@@ -3377,7 +3255,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWF</v>
@@ -3389,7 +3267,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TR</v>
@@ -3401,7 +3279,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v/>
@@ -3410,7 +3288,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>no8</v>
@@ -3422,7 +3300,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWFno8</v>
@@ -3434,7 +3312,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWFmorn</v>
@@ -3446,7 +3324,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TRmorn</v>
@@ -3458,7 +3336,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>Trmorn</v>
@@ -3470,7 +3348,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>morn</v>
@@ -3482,7 +3360,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>no8morn</v>
@@ -3494,7 +3372,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MWFno8morn</v>
@@ -3506,7 +3384,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>1:00PM4:00PM</v>
@@ -3521,7 +3399,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>1:00PM5:00PM</v>
@@ -3536,7 +3414,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>TWR1:00PM4:00PM</v>
@@ -3554,7 +3432,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>WR1:00PM4:00PM</v>
@@ -3572,7 +3450,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MT1:00PM5:00PM</v>
@@ -3590,7 +3468,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>MTW1:00PM5:00PM</v>
@@ -3608,7 +3486,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>TimeCodeMap[[#This Row],[days]]&amp;TimeCodeMap[[#This Row],[begin_time]]&amp;TimeCodeMap[[#This Row],[end_time]]</f>
         <v>ASY</v>

</xml_diff>